<commit_message>
Refactored some aspects of exceptions. Began work on ppp_input.
</commit_message>
<xml_diff>
--- a/test/FQ-nut.xlsx
+++ b/test/FQ-nut.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="0" windowWidth="27000" windowHeight="26500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6416" uniqueCount="2965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6427" uniqueCount="2976">
   <si>
     <t>type</t>
   </si>
@@ -9193,12 +9193,45 @@
   <si>
     <t>sect_non_child_nutrition_note</t>
   </si>
+  <si>
+    <t>ppp_inclusion_level</t>
+  </si>
+  <si>
+    <t>A list of regions.</t>
+  </si>
+  <si>
+    <t>A list of provinces.</t>
+  </si>
+  <si>
+    <t>A list of communes.</t>
+  </si>
+  <si>
+    <t>ppp_input::English</t>
+  </si>
+  <si>
+    <t>Une liste de régions.</t>
+  </si>
+  <si>
+    <t>Une liste de provinces.</t>
+  </si>
+  <si>
+    <t>Une liste de communes.</t>
+  </si>
+  <si>
+    <t>ppp_input::Français</t>
+  </si>
+  <si>
+    <t>A list of EAs.</t>
+  </si>
+  <si>
+    <t>Une liste de zone de ZDs.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9281,6 +9314,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -9359,7 +9404,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="597">
+  <cellStyleXfs count="609">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9957,8 +10002,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10076,8 +10133,21 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="597">
+  <cellStyles count="609">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -10376,6 +10446,12 @@
     <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -10674,6 +10750,12 @@
     <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -10971,13 +11053,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S602"/>
+  <dimension ref="A1:W602"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="U43" sqref="U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -10997,10 +11079,14 @@
     <col min="17" max="17" width="18.5" style="6" customWidth="1"/>
     <col min="18" max="18" width="19" style="6" customWidth="1"/>
     <col min="19" max="19" width="15.1640625" style="6" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="6"/>
+    <col min="20" max="20" width="3.1640625" style="6" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" style="6" customWidth="1"/>
+    <col min="22" max="22" width="15" style="6" customWidth="1"/>
+    <col min="23" max="23" width="15.83203125" style="6" customWidth="1"/>
+    <col min="24" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13" customHeight="1">
+    <row r="1" spans="1:23" ht="13" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -11058,8 +11144,18 @@
       <c r="S1" s="6" t="s">
         <v>2110</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="13" customHeight="1">
+      <c r="T1" s="7"/>
+      <c r="U1" s="7" t="s">
+        <v>2965</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>2969</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="13" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -11070,8 +11166,12 @@
         <v>17</v>
       </c>
       <c r="S2"/>
-    </row>
-    <row r="3" spans="1:19" ht="13" customHeight="1">
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+    </row>
+    <row r="3" spans="1:23" ht="13" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -11085,8 +11185,12 @@
         <v>21</v>
       </c>
       <c r="S3"/>
-    </row>
-    <row r="4" spans="1:19" ht="13" customHeight="1">
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" spans="1:23" ht="13" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -11100,8 +11204,12 @@
         <v>2126</v>
       </c>
       <c r="S4"/>
-    </row>
-    <row r="5" spans="1:19" ht="13" customHeight="1">
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+    </row>
+    <row r="5" spans="1:23" ht="13" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
@@ -11118,8 +11226,12 @@
         <v>2127</v>
       </c>
       <c r="S5"/>
-    </row>
-    <row r="6" spans="1:19" ht="13" customHeight="1">
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+    </row>
+    <row r="6" spans="1:23" ht="13" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -11127,8 +11239,12 @@
         <v>19</v>
       </c>
       <c r="S6"/>
-    </row>
-    <row r="7" spans="1:19" ht="13" customHeight="1">
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+    </row>
+    <row r="7" spans="1:23" ht="13" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -11148,8 +11264,12 @@
         <v>2128</v>
       </c>
       <c r="S7"/>
-    </row>
-    <row r="8" spans="1:19" ht="13" customHeight="1">
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+    </row>
+    <row r="8" spans="1:23" ht="13" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -11172,8 +11292,12 @@
         <v>2129</v>
       </c>
       <c r="S8"/>
-    </row>
-    <row r="9" spans="1:19" ht="13" customHeight="1">
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+    </row>
+    <row r="9" spans="1:23" ht="13" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
@@ -11196,8 +11320,12 @@
         <v>2130</v>
       </c>
       <c r="S9"/>
-    </row>
-    <row r="10" spans="1:19" ht="13" customHeight="1">
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+    </row>
+    <row r="10" spans="1:23" ht="13" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -11211,8 +11339,12 @@
         <v>44</v>
       </c>
       <c r="S10"/>
-    </row>
-    <row r="11" spans="1:19" ht="13" customHeight="1">
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+    </row>
+    <row r="11" spans="1:23" ht="13" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
@@ -11229,8 +11361,12 @@
         <v>2116</v>
       </c>
       <c r="S11"/>
-    </row>
-    <row r="12" spans="1:19" ht="13" customHeight="1">
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+    </row>
+    <row r="12" spans="1:23" ht="13" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>39</v>
       </c>
@@ -11247,8 +11383,12 @@
         <v>2117</v>
       </c>
       <c r="S12"/>
-    </row>
-    <row r="13" spans="1:19" ht="13" customHeight="1">
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+    </row>
+    <row r="13" spans="1:23" ht="13" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
@@ -11265,8 +11405,12 @@
         <v>2118</v>
       </c>
       <c r="S13"/>
-    </row>
-    <row r="14" spans="1:19" ht="13" customHeight="1">
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+    </row>
+    <row r="14" spans="1:23" ht="13" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>39</v>
       </c>
@@ -11283,8 +11427,12 @@
         <v>2119</v>
       </c>
       <c r="S14"/>
-    </row>
-    <row r="15" spans="1:19" ht="13" customHeight="1">
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+    </row>
+    <row r="15" spans="1:23" ht="13" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -11304,8 +11452,12 @@
         <v>2131</v>
       </c>
       <c r="S15"/>
-    </row>
-    <row r="16" spans="1:19" ht="13" customHeight="1">
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+    </row>
+    <row r="16" spans="1:23" ht="13" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
@@ -11325,8 +11477,12 @@
         <v>2132</v>
       </c>
       <c r="S16"/>
-    </row>
-    <row r="17" spans="1:19" ht="13" customHeight="1">
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+    </row>
+    <row r="17" spans="1:23" ht="13" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
@@ -11334,8 +11490,12 @@
         <v>43</v>
       </c>
       <c r="S17"/>
-    </row>
-    <row r="18" spans="1:19" ht="13" customHeight="1">
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+    </row>
+    <row r="18" spans="1:23" ht="13" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
@@ -11346,8 +11506,12 @@
         <v>2114</v>
       </c>
       <c r="S18"/>
-    </row>
-    <row r="19" spans="1:19" ht="13" customHeight="1">
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+    </row>
+    <row r="19" spans="1:23" ht="13" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
@@ -11358,8 +11522,12 @@
         <v>20</v>
       </c>
       <c r="S19"/>
-    </row>
-    <row r="20" spans="1:19" ht="13" customHeight="1">
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+    </row>
+    <row r="20" spans="1:23" ht="13" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
@@ -11385,8 +11553,12 @@
         <v>2134</v>
       </c>
       <c r="S20"/>
-    </row>
-    <row r="21" spans="1:19" ht="13" customHeight="1">
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+    </row>
+    <row r="21" spans="1:23" ht="13" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
@@ -11403,8 +11575,12 @@
         <v>2135</v>
       </c>
       <c r="S21"/>
-    </row>
-    <row r="22" spans="1:19" ht="13" customHeight="1">
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+    </row>
+    <row r="22" spans="1:23" ht="13" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -11421,8 +11597,12 @@
         <v>2136</v>
       </c>
       <c r="S22"/>
-    </row>
-    <row r="23" spans="1:19" ht="13" customHeight="1">
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+    </row>
+    <row r="23" spans="1:23" ht="13" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -11439,8 +11619,12 @@
         <v>69</v>
       </c>
       <c r="S23"/>
-    </row>
-    <row r="24" spans="1:19" ht="13" customHeight="1">
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+    </row>
+    <row r="24" spans="1:23" ht="13" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
@@ -11448,8 +11632,12 @@
         <v>57</v>
       </c>
       <c r="S24"/>
-    </row>
-    <row r="25" spans="1:19" ht="13" customHeight="1">
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+    </row>
+    <row r="25" spans="1:23" ht="13" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -11460,8 +11648,12 @@
         <v>20</v>
       </c>
       <c r="S25"/>
-    </row>
-    <row r="26" spans="1:19" ht="13" customHeight="1">
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+    </row>
+    <row r="26" spans="1:23" ht="13" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>39</v>
       </c>
@@ -11481,8 +11673,12 @@
         <v>2867</v>
       </c>
       <c r="S26"/>
-    </row>
-    <row r="27" spans="1:19" ht="13" customHeight="1">
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+    </row>
+    <row r="27" spans="1:23" ht="13" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>30</v>
       </c>
@@ -11502,8 +11698,12 @@
         <v>2868</v>
       </c>
       <c r="S27"/>
-    </row>
-    <row r="28" spans="1:19" ht="13" customHeight="1">
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+    </row>
+    <row r="28" spans="1:23" ht="13" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>29</v>
       </c>
@@ -11511,8 +11711,12 @@
         <v>70</v>
       </c>
       <c r="S28"/>
-    </row>
-    <row r="29" spans="1:19" ht="13" customHeight="1">
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+    </row>
+    <row r="29" spans="1:23" ht="13" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>39</v>
       </c>
@@ -11538,8 +11742,12 @@
         <v>2870</v>
       </c>
       <c r="S29"/>
-    </row>
-    <row r="30" spans="1:19" ht="13" customHeight="1">
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+    </row>
+    <row r="30" spans="1:23" ht="13" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>15</v>
       </c>
@@ -11550,8 +11758,12 @@
         <v>78</v>
       </c>
       <c r="S30"/>
-    </row>
-    <row r="31" spans="1:19" ht="13" customHeight="1">
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+    </row>
+    <row r="31" spans="1:23" ht="13" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>18</v>
       </c>
@@ -11565,8 +11777,12 @@
         <v>2112</v>
       </c>
       <c r="S31"/>
-    </row>
-    <row r="32" spans="1:19" ht="13" customHeight="1">
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+    </row>
+    <row r="32" spans="1:23" ht="13" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>80</v>
       </c>
@@ -11586,8 +11802,12 @@
         <v>2137</v>
       </c>
       <c r="S32"/>
-    </row>
-    <row r="33" spans="1:19" ht="13" customHeight="1">
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+    </row>
+    <row r="33" spans="1:23" ht="13" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>30</v>
       </c>
@@ -11604,8 +11824,12 @@
         <v>2138</v>
       </c>
       <c r="S33"/>
-    </row>
-    <row r="34" spans="1:19" ht="13" customHeight="1">
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+    </row>
+    <row r="34" spans="1:23" ht="13" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
@@ -11613,8 +11837,12 @@
         <v>79</v>
       </c>
       <c r="S34"/>
-    </row>
-    <row r="35" spans="1:19" ht="13" customHeight="1">
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+    </row>
+    <row r="35" spans="1:23" ht="13" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>80</v>
       </c>
@@ -11646,8 +11874,12 @@
         <v>2359</v>
       </c>
       <c r="S35"/>
-    </row>
-    <row r="36" spans="1:19" ht="13" customHeight="1">
+      <c r="T35" s="48"/>
+      <c r="U35" s="48"/>
+      <c r="V35" s="48"/>
+      <c r="W35" s="48"/>
+    </row>
+    <row r="36" spans="1:23" ht="13" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>15</v>
       </c>
@@ -11658,8 +11890,12 @@
         <v>89</v>
       </c>
       <c r="S36"/>
-    </row>
-    <row r="37" spans="1:19" ht="13" customHeight="1">
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+    </row>
+    <row r="37" spans="1:23" ht="13" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>18</v>
       </c>
@@ -11670,8 +11906,12 @@
         <v>20</v>
       </c>
       <c r="S37"/>
-    </row>
-    <row r="38" spans="1:19" ht="13" customHeight="1">
+      <c r="T37" s="48"/>
+      <c r="U37" s="48"/>
+      <c r="V37" s="48"/>
+      <c r="W37" s="48"/>
+    </row>
+    <row r="38" spans="1:23" ht="13" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>22</v>
       </c>
@@ -11688,8 +11928,12 @@
         <v>2140</v>
       </c>
       <c r="S38"/>
-    </row>
-    <row r="39" spans="1:19" ht="13" customHeight="1">
+      <c r="T38" s="48"/>
+      <c r="U38" s="48"/>
+      <c r="V38" s="48"/>
+      <c r="W38" s="48"/>
+    </row>
+    <row r="39" spans="1:23" ht="13" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>22</v>
       </c>
@@ -11706,8 +11950,12 @@
         <v>2140</v>
       </c>
       <c r="S39"/>
-    </row>
-    <row r="40" spans="1:19" ht="13" customHeight="1">
+      <c r="T39" s="48"/>
+      <c r="U39" s="48"/>
+      <c r="V39" s="48"/>
+      <c r="W39" s="48"/>
+    </row>
+    <row r="40" spans="1:23" ht="13" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>39</v>
       </c>
@@ -11724,8 +11972,16 @@
         <v>2121</v>
       </c>
       <c r="S40"/>
-    </row>
-    <row r="41" spans="1:19" ht="13" customHeight="1">
+      <c r="T40" s="48"/>
+      <c r="U40" s="48"/>
+      <c r="V40" s="48" t="s">
+        <v>2966</v>
+      </c>
+      <c r="W40" s="48" t="s">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="13" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>39</v>
       </c>
@@ -11742,8 +11998,16 @@
         <v>2122</v>
       </c>
       <c r="S41"/>
-    </row>
-    <row r="42" spans="1:19" ht="13" customHeight="1">
+      <c r="T41" s="48"/>
+      <c r="U41" s="48"/>
+      <c r="V41" s="48" t="s">
+        <v>2967</v>
+      </c>
+      <c r="W41" s="48" t="s">
+        <v>2971</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" ht="13" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>39</v>
       </c>
@@ -11760,8 +12024,16 @@
         <v>2123</v>
       </c>
       <c r="S42"/>
-    </row>
-    <row r="43" spans="1:19" ht="13" customHeight="1">
+      <c r="T42" s="47"/>
+      <c r="U42" s="47"/>
+      <c r="V42" s="48" t="s">
+        <v>2968</v>
+      </c>
+      <c r="W42" s="48" t="s">
+        <v>2972</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="13" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>39</v>
       </c>
@@ -11778,8 +12050,16 @@
         <v>2124</v>
       </c>
       <c r="S43"/>
-    </row>
-    <row r="44" spans="1:19" ht="13" customHeight="1">
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7" t="s">
+        <v>2974</v>
+      </c>
+      <c r="W43" s="48" t="s">
+        <v>2975</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="13" customHeight="1">
       <c r="A44" s="6" t="s">
         <v>50</v>
       </c>
@@ -11796,8 +12076,11 @@
         <v>2141</v>
       </c>
       <c r="S44"/>
-    </row>
-    <row r="45" spans="1:19" ht="13" customHeight="1">
+      <c r="T44" s="7"/>
+      <c r="U44" s="7"/>
+      <c r="V44" s="7"/>
+    </row>
+    <row r="45" spans="1:23" ht="13" customHeight="1">
       <c r="A45" s="6" t="s">
         <v>50</v>
       </c>
@@ -11814,8 +12097,11 @@
         <v>2142</v>
       </c>
       <c r="S45"/>
-    </row>
-    <row r="46" spans="1:19" ht="13" customHeight="1">
+      <c r="T45" s="48"/>
+      <c r="U45" s="48"/>
+      <c r="V45" s="48"/>
+    </row>
+    <row r="46" spans="1:23" ht="13" customHeight="1">
       <c r="A46" s="6" t="s">
         <v>30</v>
       </c>
@@ -11841,8 +12127,11 @@
         <v>2144</v>
       </c>
       <c r="S46"/>
-    </row>
-    <row r="47" spans="1:19" ht="13" customHeight="1">
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+    </row>
+    <row r="47" spans="1:23" ht="13" customHeight="1">
       <c r="A47" s="6" t="s">
         <v>29</v>
       </c>
@@ -11850,8 +12139,11 @@
         <v>90</v>
       </c>
       <c r="S47"/>
-    </row>
-    <row r="48" spans="1:19" ht="13" customHeight="1">
+      <c r="T47" s="48"/>
+      <c r="U47" s="48"/>
+      <c r="V47" s="48"/>
+    </row>
+    <row r="48" spans="1:23" ht="13" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>30</v>
       </c>
@@ -11886,8 +12178,11 @@
         <v>2147</v>
       </c>
       <c r="S48"/>
-    </row>
-    <row r="49" spans="1:19" ht="13" customHeight="1">
+      <c r="T48" s="48"/>
+      <c r="U48" s="48"/>
+      <c r="V48" s="48"/>
+    </row>
+    <row r="49" spans="1:22" ht="13" customHeight="1">
       <c r="A49" s="6" t="s">
         <v>30</v>
       </c>
@@ -11904,8 +12199,11 @@
         <v>2148</v>
       </c>
       <c r="S49"/>
-    </row>
-    <row r="50" spans="1:19" ht="13" customHeight="1">
+      <c r="T49" s="48"/>
+      <c r="U49" s="48"/>
+      <c r="V49" s="48"/>
+    </row>
+    <row r="50" spans="1:22" ht="13" customHeight="1">
       <c r="A50" s="6" t="s">
         <v>114</v>
       </c>
@@ -11925,8 +12223,11 @@
         <v>2149</v>
       </c>
       <c r="S50"/>
-    </row>
-    <row r="51" spans="1:19" ht="13" customHeight="1">
+      <c r="T50" s="48"/>
+      <c r="U50" s="48"/>
+      <c r="V50" s="48"/>
+    </row>
+    <row r="51" spans="1:22" ht="13" customHeight="1">
       <c r="A51" s="6" t="s">
         <v>22</v>
       </c>
@@ -11952,8 +12253,11 @@
         <v>2828</v>
       </c>
       <c r="S51"/>
-    </row>
-    <row r="52" spans="1:19" ht="13" customHeight="1">
+      <c r="T51" s="48"/>
+      <c r="U51" s="48"/>
+      <c r="V51" s="48"/>
+    </row>
+    <row r="52" spans="1:22" ht="13" customHeight="1">
       <c r="A52" s="6" t="s">
         <v>22</v>
       </c>
@@ -11973,8 +12277,11 @@
         <v>2827</v>
       </c>
       <c r="S52"/>
-    </row>
-    <row r="53" spans="1:19" ht="13" customHeight="1">
+      <c r="T52" s="47"/>
+      <c r="U52" s="47"/>
+      <c r="V52" s="49"/>
+    </row>
+    <row r="53" spans="1:22" ht="13" customHeight="1">
       <c r="A53" s="6" t="s">
         <v>30</v>
       </c>
@@ -11994,8 +12301,11 @@
         <v>2151</v>
       </c>
       <c r="S53"/>
-    </row>
-    <row r="54" spans="1:19" ht="13" customHeight="1">
+      <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
+      <c r="V53" s="7"/>
+    </row>
+    <row r="54" spans="1:22" ht="13" customHeight="1">
       <c r="A54" s="6" t="s">
         <v>18</v>
       </c>
@@ -12009,8 +12319,11 @@
         <v>126</v>
       </c>
       <c r="S54"/>
-    </row>
-    <row r="55" spans="1:19" ht="13" customHeight="1">
+      <c r="T54" s="7"/>
+      <c r="U54" s="7"/>
+      <c r="V54" s="7"/>
+    </row>
+    <row r="55" spans="1:22" ht="13" customHeight="1">
       <c r="A55" s="6" t="s">
         <v>34</v>
       </c>
@@ -12033,8 +12346,11 @@
         <v>2153</v>
       </c>
       <c r="S55"/>
-    </row>
-    <row r="56" spans="1:19" ht="13" customHeight="1">
+      <c r="T55" s="7"/>
+      <c r="U55" s="7"/>
+      <c r="V55" s="7"/>
+    </row>
+    <row r="56" spans="1:22" ht="13" customHeight="1">
       <c r="A56" s="6" t="s">
         <v>130</v>
       </c>
@@ -12048,8 +12364,11 @@
         <v>2154</v>
       </c>
       <c r="S56"/>
-    </row>
-    <row r="57" spans="1:19" ht="13" customHeight="1">
+      <c r="T56" s="50"/>
+      <c r="U56" s="50"/>
+      <c r="V56" s="50"/>
+    </row>
+    <row r="57" spans="1:22" ht="13" customHeight="1">
       <c r="A57" s="6" t="s">
         <v>29</v>
       </c>
@@ -12057,8 +12376,11 @@
         <v>125</v>
       </c>
       <c r="S57"/>
-    </row>
-    <row r="58" spans="1:19" ht="13" customHeight="1">
+      <c r="T57" s="50"/>
+      <c r="U57" s="50"/>
+      <c r="V57" s="50"/>
+    </row>
+    <row r="58" spans="1:22" ht="13" customHeight="1">
       <c r="A58" s="6" t="s">
         <v>15</v>
       </c>
@@ -12069,8 +12391,11 @@
         <v>134</v>
       </c>
       <c r="S58"/>
-    </row>
-    <row r="59" spans="1:19" ht="13" customHeight="1">
+      <c r="T58" s="50"/>
+      <c r="U58" s="50"/>
+      <c r="V58" s="50"/>
+    </row>
+    <row r="59" spans="1:22" ht="13" customHeight="1">
       <c r="A59" s="6" t="s">
         <v>22</v>
       </c>
@@ -12096,8 +12421,11 @@
         <v>2670</v>
       </c>
       <c r="S59"/>
-    </row>
-    <row r="60" spans="1:19" ht="13" customHeight="1">
+      <c r="T59" s="50"/>
+      <c r="U59" s="50"/>
+      <c r="V59" s="50"/>
+    </row>
+    <row r="60" spans="1:22" ht="13" customHeight="1">
       <c r="A60" s="6" t="s">
         <v>130</v>
       </c>
@@ -12125,8 +12453,11 @@
       </c>
       <c r="R60" s="45"/>
       <c r="S60"/>
-    </row>
-    <row r="61" spans="1:19" ht="13" customHeight="1">
+      <c r="T60" s="50"/>
+      <c r="U60" s="50"/>
+      <c r="V60" s="50"/>
+    </row>
+    <row r="61" spans="1:22" ht="13" customHeight="1">
       <c r="A61" s="6" t="s">
         <v>39</v>
       </c>
@@ -12157,8 +12488,11 @@
         <v>2876</v>
       </c>
       <c r="S61"/>
-    </row>
-    <row r="62" spans="1:19" ht="13" customHeight="1">
+      <c r="T61" s="50"/>
+      <c r="U61" s="50"/>
+      <c r="V61" s="50"/>
+    </row>
+    <row r="62" spans="1:22" ht="13" customHeight="1">
       <c r="A62" s="6" t="s">
         <v>39</v>
       </c>
@@ -12181,8 +12515,11 @@
         <v>2156</v>
       </c>
       <c r="S62"/>
-    </row>
-    <row r="63" spans="1:19" ht="13" customHeight="1">
+      <c r="T62" s="50"/>
+      <c r="U62" s="50"/>
+      <c r="V62" s="50"/>
+    </row>
+    <row r="63" spans="1:22" ht="13" customHeight="1">
       <c r="A63" s="6" t="s">
         <v>15</v>
       </c>
@@ -12193,11 +12530,17 @@
         <v>148</v>
       </c>
       <c r="S63"/>
-    </row>
-    <row r="64" spans="1:19" ht="13" customHeight="1">
+      <c r="T63" s="50"/>
+      <c r="U63" s="50"/>
+      <c r="V63" s="50"/>
+    </row>
+    <row r="64" spans="1:22" ht="13" customHeight="1">
       <c r="S64"/>
-    </row>
-    <row r="65" spans="1:19" s="11" customFormat="1" ht="13" customHeight="1">
+      <c r="T64" s="50"/>
+      <c r="U64" s="50"/>
+      <c r="V64" s="50"/>
+    </row>
+    <row r="65" spans="1:22" s="11" customFormat="1" ht="13" customHeight="1">
       <c r="A65" s="11" t="s">
         <v>22</v>
       </c>
@@ -12224,8 +12567,11 @@
       </c>
       <c r="R65" s="6"/>
       <c r="S65"/>
-    </row>
-    <row r="66" spans="1:19" ht="13" customHeight="1">
+      <c r="T65" s="50"/>
+      <c r="U65" s="50"/>
+      <c r="V65" s="50"/>
+    </row>
+    <row r="66" spans="1:22" ht="13" customHeight="1">
       <c r="A66" s="6" t="s">
         <v>18</v>
       </c>
@@ -12239,8 +12585,11 @@
         <v>151</v>
       </c>
       <c r="S66"/>
-    </row>
-    <row r="67" spans="1:19" ht="13" customHeight="1">
+      <c r="T66" s="50"/>
+      <c r="U66" s="50"/>
+      <c r="V66" s="50"/>
+    </row>
+    <row r="67" spans="1:22" ht="13" customHeight="1">
       <c r="A67" s="6" t="s">
         <v>22</v>
       </c>
@@ -12257,8 +12606,11 @@
         <v>2159</v>
       </c>
       <c r="S67"/>
-    </row>
-    <row r="68" spans="1:19" ht="13" customHeight="1">
+      <c r="T67" s="50"/>
+      <c r="U67" s="50"/>
+      <c r="V67" s="50"/>
+    </row>
+    <row r="68" spans="1:22" ht="13" customHeight="1">
       <c r="A68" s="6" t="s">
         <v>22</v>
       </c>
@@ -12275,8 +12627,11 @@
         <v>2160</v>
       </c>
       <c r="S68"/>
-    </row>
-    <row r="69" spans="1:19" ht="13" customHeight="1">
+      <c r="T68" s="50"/>
+      <c r="U68" s="50"/>
+      <c r="V68" s="50"/>
+    </row>
+    <row r="69" spans="1:22" ht="13" customHeight="1">
       <c r="A69" s="6" t="s">
         <v>157</v>
       </c>
@@ -12308,8 +12663,11 @@
         <v>2161</v>
       </c>
       <c r="S69"/>
-    </row>
-    <row r="70" spans="1:19" ht="13" customHeight="1">
+      <c r="T69" s="50"/>
+      <c r="U69" s="50"/>
+      <c r="V69" s="50"/>
+    </row>
+    <row r="70" spans="1:22" ht="13" customHeight="1">
       <c r="A70" s="6" t="s">
         <v>29</v>
       </c>
@@ -12317,8 +12675,11 @@
         <v>152</v>
       </c>
       <c r="S70"/>
-    </row>
-    <row r="71" spans="1:19" ht="13" customHeight="1">
+      <c r="T70" s="50"/>
+      <c r="U70" s="50"/>
+      <c r="V70" s="50"/>
+    </row>
+    <row r="71" spans="1:22" ht="13" customHeight="1">
       <c r="A71" s="6" t="s">
         <v>15</v>
       </c>
@@ -12329,8 +12690,11 @@
         <v>164</v>
       </c>
       <c r="S71"/>
-    </row>
-    <row r="72" spans="1:19" ht="13" customHeight="1">
+      <c r="T71" s="50"/>
+      <c r="U71" s="50"/>
+      <c r="V71" s="50"/>
+    </row>
+    <row r="72" spans="1:22" ht="13" customHeight="1">
       <c r="A72" s="6" t="s">
         <v>15</v>
       </c>
@@ -12341,8 +12705,11 @@
         <v>166</v>
       </c>
       <c r="S72"/>
-    </row>
-    <row r="73" spans="1:19" ht="13" customHeight="1">
+      <c r="T72" s="50"/>
+      <c r="U72" s="50"/>
+      <c r="V72" s="50"/>
+    </row>
+    <row r="73" spans="1:22" ht="13" customHeight="1">
       <c r="A73" s="6" t="s">
         <v>15</v>
       </c>
@@ -12353,8 +12720,11 @@
         <v>168</v>
       </c>
       <c r="S73"/>
-    </row>
-    <row r="74" spans="1:19" ht="13" customHeight="1">
+      <c r="T73" s="50"/>
+      <c r="U73" s="50"/>
+      <c r="V73" s="50"/>
+    </row>
+    <row r="74" spans="1:22" ht="13" customHeight="1">
       <c r="A74" s="6" t="s">
         <v>15</v>
       </c>
@@ -12365,8 +12735,11 @@
         <v>170</v>
       </c>
       <c r="S74"/>
-    </row>
-    <row r="75" spans="1:19" ht="13" customHeight="1">
+      <c r="T74" s="50"/>
+      <c r="U74" s="50"/>
+      <c r="V74" s="50"/>
+    </row>
+    <row r="75" spans="1:22" ht="13" customHeight="1">
       <c r="A75" s="6" t="s">
         <v>50</v>
       </c>
@@ -12395,8 +12768,11 @@
         <v>2830</v>
       </c>
       <c r="S75"/>
-    </row>
-    <row r="76" spans="1:19" ht="13" customHeight="1">
+      <c r="T75" s="50"/>
+      <c r="U75" s="50"/>
+      <c r="V75" s="50"/>
+    </row>
+    <row r="76" spans="1:22" ht="13" customHeight="1">
       <c r="A76" s="6" t="s">
         <v>18</v>
       </c>
@@ -12413,8 +12789,11 @@
         <v>2909</v>
       </c>
       <c r="S76"/>
-    </row>
-    <row r="77" spans="1:19" ht="13" customHeight="1">
+      <c r="T76" s="50"/>
+      <c r="U76" s="50"/>
+      <c r="V76" s="50"/>
+    </row>
+    <row r="77" spans="1:22" ht="13" customHeight="1">
       <c r="A77" s="6" t="s">
         <v>22</v>
       </c>
@@ -12431,8 +12810,11 @@
         <v>2882</v>
       </c>
       <c r="S77"/>
-    </row>
-    <row r="78" spans="1:19" ht="13" customHeight="1">
+      <c r="T77" s="50"/>
+      <c r="U77" s="50"/>
+      <c r="V77" s="50"/>
+    </row>
+    <row r="78" spans="1:22" ht="13" customHeight="1">
       <c r="A78" s="6" t="s">
         <v>22</v>
       </c>
@@ -12449,8 +12831,11 @@
         <v>2163</v>
       </c>
       <c r="S78"/>
-    </row>
-    <row r="79" spans="1:19" ht="13" customHeight="1">
+      <c r="T78" s="50"/>
+      <c r="U78" s="50"/>
+      <c r="V78" s="50"/>
+    </row>
+    <row r="79" spans="1:22" ht="13" customHeight="1">
       <c r="A79" s="6" t="s">
         <v>22</v>
       </c>
@@ -12467,8 +12852,11 @@
         <v>2164</v>
       </c>
       <c r="S79"/>
-    </row>
-    <row r="80" spans="1:19" ht="13" customHeight="1">
+      <c r="T79" s="50"/>
+      <c r="U79" s="50"/>
+      <c r="V79" s="50"/>
+    </row>
+    <row r="80" spans="1:22" ht="13" customHeight="1">
       <c r="A80" s="6" t="s">
         <v>50</v>
       </c>
@@ -12494,8 +12882,11 @@
         <v>2165</v>
       </c>
       <c r="S80"/>
-    </row>
-    <row r="81" spans="1:19" ht="13" customHeight="1">
+      <c r="T80" s="50"/>
+      <c r="U80" s="50"/>
+      <c r="V80" s="50"/>
+    </row>
+    <row r="81" spans="1:22" ht="13" customHeight="1">
       <c r="A81" s="6" t="s">
         <v>15</v>
       </c>
@@ -12506,8 +12897,11 @@
         <v>187</v>
       </c>
       <c r="S81"/>
-    </row>
-    <row r="82" spans="1:19" ht="13" customHeight="1">
+      <c r="T81" s="50"/>
+      <c r="U81" s="50"/>
+      <c r="V81" s="50"/>
+    </row>
+    <row r="82" spans="1:22" ht="13" customHeight="1">
       <c r="A82" s="6" t="s">
         <v>15</v>
       </c>
@@ -12518,8 +12912,11 @@
         <v>189</v>
       </c>
       <c r="S82"/>
-    </row>
-    <row r="83" spans="1:19" ht="13" customHeight="1">
+      <c r="T82" s="50"/>
+      <c r="U82" s="50"/>
+      <c r="V82" s="50"/>
+    </row>
+    <row r="83" spans="1:22" ht="13" customHeight="1">
       <c r="A83" s="6" t="s">
         <v>15</v>
       </c>
@@ -12530,8 +12927,11 @@
         <v>191</v>
       </c>
       <c r="S83"/>
-    </row>
-    <row r="84" spans="1:19" ht="13" customHeight="1">
+      <c r="T83" s="50"/>
+      <c r="U83" s="50"/>
+      <c r="V83" s="50"/>
+    </row>
+    <row r="84" spans="1:22" ht="13" customHeight="1">
       <c r="A84" s="6" t="s">
         <v>29</v>
       </c>
@@ -12539,8 +12939,11 @@
         <v>175</v>
       </c>
       <c r="S84"/>
-    </row>
-    <row r="85" spans="1:19" ht="13" customHeight="1">
+      <c r="T84" s="50"/>
+      <c r="U84" s="50"/>
+      <c r="V84" s="50"/>
+    </row>
+    <row r="85" spans="1:22" ht="13" customHeight="1">
       <c r="A85" s="6" t="s">
         <v>192</v>
       </c>
@@ -12560,8 +12963,11 @@
         <v>2166</v>
       </c>
       <c r="S85"/>
-    </row>
-    <row r="86" spans="1:19" ht="13" customHeight="1">
+      <c r="T85" s="50"/>
+      <c r="U85" s="50"/>
+      <c r="V85" s="50"/>
+    </row>
+    <row r="86" spans="1:22" ht="13" customHeight="1">
       <c r="A86" s="6" t="s">
         <v>195</v>
       </c>
@@ -12581,8 +12987,11 @@
         <v>2167</v>
       </c>
       <c r="S86"/>
-    </row>
-    <row r="87" spans="1:19" ht="13" customHeight="1">
+      <c r="T86" s="50"/>
+      <c r="U86" s="50"/>
+      <c r="V86" s="50"/>
+    </row>
+    <row r="87" spans="1:22" ht="13" customHeight="1">
       <c r="A87" s="6" t="s">
         <v>198</v>
       </c>
@@ -12602,8 +13011,11 @@
         <v>2168</v>
       </c>
       <c r="S87"/>
-    </row>
-    <row r="88" spans="1:19" ht="13" customHeight="1">
+      <c r="T87" s="50"/>
+      <c r="U87" s="50"/>
+      <c r="V87" s="50"/>
+    </row>
+    <row r="88" spans="1:22" ht="13" customHeight="1">
       <c r="A88" s="6" t="s">
         <v>201</v>
       </c>
@@ -12623,8 +13035,11 @@
         <v>2169</v>
       </c>
       <c r="S88"/>
-    </row>
-    <row r="89" spans="1:19" ht="13" customHeight="1">
+      <c r="T88" s="7"/>
+      <c r="U88" s="7"/>
+      <c r="V88" s="7"/>
+    </row>
+    <row r="89" spans="1:22" ht="13" customHeight="1">
       <c r="A89" s="6" t="s">
         <v>118</v>
       </c>
@@ -12644,8 +13059,11 @@
         <v>2170</v>
       </c>
       <c r="S89"/>
-    </row>
-    <row r="90" spans="1:19" ht="13" customHeight="1">
+      <c r="T89" s="7"/>
+      <c r="U89" s="7"/>
+      <c r="V89" s="7"/>
+    </row>
+    <row r="90" spans="1:22" ht="13" customHeight="1">
       <c r="A90" s="6" t="s">
         <v>208</v>
       </c>
@@ -12665,8 +13083,11 @@
         <v>2171</v>
       </c>
       <c r="S90"/>
-    </row>
-    <row r="91" spans="1:19" ht="13" customHeight="1">
+      <c r="T90" s="7"/>
+      <c r="U90" s="7"/>
+      <c r="V90" s="7"/>
+    </row>
+    <row r="91" spans="1:22" ht="13" customHeight="1">
       <c r="A91" s="6" t="s">
         <v>195</v>
       </c>
@@ -12686,8 +13107,11 @@
         <v>2172</v>
       </c>
       <c r="S91"/>
-    </row>
-    <row r="92" spans="1:19" ht="13" customHeight="1">
+      <c r="T91" s="7"/>
+      <c r="U91" s="7"/>
+      <c r="V91" s="7"/>
+    </row>
+    <row r="92" spans="1:22" ht="13" customHeight="1">
       <c r="A92" s="6" t="s">
         <v>50</v>
       </c>
@@ -12722,8 +13146,11 @@
         <v>2696</v>
       </c>
       <c r="S92"/>
-    </row>
-    <row r="93" spans="1:19" ht="13" customHeight="1">
+      <c r="T92" s="7"/>
+      <c r="U92" s="7"/>
+      <c r="V92" s="7"/>
+    </row>
+    <row r="93" spans="1:22" ht="13" customHeight="1">
       <c r="A93" s="6" t="s">
         <v>118</v>
       </c>
@@ -12743,8 +13170,11 @@
         <v>2175</v>
       </c>
       <c r="S93"/>
-    </row>
-    <row r="94" spans="1:19" ht="13" customHeight="1">
+      <c r="T93" s="7"/>
+      <c r="U93" s="7"/>
+      <c r="V93" s="7"/>
+    </row>
+    <row r="94" spans="1:22" ht="13" customHeight="1">
       <c r="A94" s="6" t="s">
         <v>22</v>
       </c>
@@ -12764,8 +13194,11 @@
         <v>2176</v>
       </c>
       <c r="S94"/>
-    </row>
-    <row r="95" spans="1:19" ht="13" customHeight="1">
+      <c r="T94" s="7"/>
+      <c r="U94" s="7"/>
+      <c r="V94" s="7"/>
+    </row>
+    <row r="95" spans="1:22" ht="13" customHeight="1">
       <c r="A95" s="6" t="s">
         <v>157</v>
       </c>
@@ -12806,8 +13239,11 @@
         <v>2179</v>
       </c>
       <c r="S95"/>
-    </row>
-    <row r="96" spans="1:19" ht="13" customHeight="1">
+      <c r="T95" s="7"/>
+      <c r="U95" s="7"/>
+      <c r="V95" s="7"/>
+    </row>
+    <row r="96" spans="1:22" ht="13" customHeight="1">
       <c r="A96" s="6" t="s">
         <v>15</v>
       </c>
@@ -12821,8 +13257,11 @@
         <v>233</v>
       </c>
       <c r="S96"/>
-    </row>
-    <row r="97" spans="1:19" ht="13" customHeight="1">
+      <c r="T96" s="7"/>
+      <c r="U96" s="7"/>
+      <c r="V96" s="7"/>
+    </row>
+    <row r="97" spans="1:22" ht="13" customHeight="1">
       <c r="A97" s="6" t="s">
         <v>15</v>
       </c>
@@ -12833,8 +13272,11 @@
         <v>235</v>
       </c>
       <c r="S97"/>
-    </row>
-    <row r="98" spans="1:19" ht="13" customHeight="1">
+      <c r="T97" s="7"/>
+      <c r="U97" s="7"/>
+      <c r="V97" s="7"/>
+    </row>
+    <row r="98" spans="1:22" ht="13" customHeight="1">
       <c r="A98" s="6" t="s">
         <v>15</v>
       </c>
@@ -12845,8 +13287,11 @@
         <v>237</v>
       </c>
       <c r="S98"/>
-    </row>
-    <row r="99" spans="1:19" ht="13" customHeight="1">
+      <c r="T98" s="7"/>
+      <c r="U98" s="7"/>
+      <c r="V98" s="7"/>
+    </row>
+    <row r="99" spans="1:22" ht="13" customHeight="1">
       <c r="A99" s="6" t="s">
         <v>157</v>
       </c>
@@ -12887,8 +13332,11 @@
         <v>2180</v>
       </c>
       <c r="S99"/>
-    </row>
-    <row r="100" spans="1:19" ht="13" customHeight="1">
+      <c r="T99" s="7"/>
+      <c r="U99" s="7"/>
+      <c r="V99" s="7"/>
+    </row>
+    <row r="100" spans="1:22" ht="13" customHeight="1">
       <c r="A100" s="6" t="s">
         <v>15</v>
       </c>
@@ -12902,8 +13350,11 @@
         <v>245</v>
       </c>
       <c r="S100"/>
-    </row>
-    <row r="101" spans="1:19" ht="13" customHeight="1">
+      <c r="T100" s="7"/>
+      <c r="U100" s="7"/>
+      <c r="V100" s="7"/>
+    </row>
+    <row r="101" spans="1:22" ht="13" customHeight="1">
       <c r="A101" s="6" t="s">
         <v>15</v>
       </c>
@@ -12917,8 +13368,11 @@
         <v>247</v>
       </c>
       <c r="S101"/>
-    </row>
-    <row r="102" spans="1:19" ht="13" customHeight="1">
+      <c r="T101" s="48"/>
+      <c r="U101" s="48"/>
+      <c r="V101" s="48"/>
+    </row>
+    <row r="102" spans="1:22" ht="13" customHeight="1">
       <c r="A102" s="6" t="s">
         <v>15</v>
       </c>
@@ -12932,8 +13386,11 @@
         <v>249</v>
       </c>
       <c r="S102"/>
-    </row>
-    <row r="103" spans="1:19" ht="13" customHeight="1">
+      <c r="T102" s="7"/>
+      <c r="U102" s="7"/>
+      <c r="V102" s="7"/>
+    </row>
+    <row r="103" spans="1:22" ht="13" customHeight="1">
       <c r="A103" s="6" t="s">
         <v>15</v>
       </c>
@@ -12947,8 +13404,11 @@
         <v>251</v>
       </c>
       <c r="S103"/>
-    </row>
-    <row r="104" spans="1:19" ht="13" customHeight="1">
+      <c r="T103" s="48"/>
+      <c r="U103" s="48"/>
+      <c r="V103" s="48"/>
+    </row>
+    <row r="104" spans="1:22" ht="13" customHeight="1">
       <c r="A104" s="6" t="s">
         <v>15</v>
       </c>
@@ -12962,8 +13422,11 @@
         <v>253</v>
       </c>
       <c r="S104"/>
-    </row>
-    <row r="105" spans="1:19" ht="13" customHeight="1">
+      <c r="T104" s="48"/>
+      <c r="U104" s="48"/>
+      <c r="V104" s="48"/>
+    </row>
+    <row r="105" spans="1:22" ht="13" customHeight="1">
       <c r="A105" s="6" t="s">
         <v>15</v>
       </c>
@@ -12977,8 +13440,11 @@
         <v>255</v>
       </c>
       <c r="S105"/>
-    </row>
-    <row r="106" spans="1:19" ht="13" customHeight="1">
+      <c r="T105" s="48"/>
+      <c r="U105" s="48"/>
+      <c r="V105" s="48"/>
+    </row>
+    <row r="106" spans="1:22" ht="13" customHeight="1">
       <c r="A106" s="6" t="s">
         <v>15</v>
       </c>
@@ -12992,8 +13458,11 @@
         <v>257</v>
       </c>
       <c r="S106"/>
-    </row>
-    <row r="107" spans="1:19" ht="13" customHeight="1">
+      <c r="T106" s="48"/>
+      <c r="U106" s="48"/>
+      <c r="V106" s="48"/>
+    </row>
+    <row r="107" spans="1:22" ht="13" customHeight="1">
       <c r="A107" s="6" t="s">
         <v>15</v>
       </c>
@@ -13007,8 +13476,11 @@
         <v>259</v>
       </c>
       <c r="S107"/>
-    </row>
-    <row r="108" spans="1:19" ht="13" customHeight="1">
+      <c r="T107" s="48"/>
+      <c r="U107" s="48"/>
+      <c r="V107" s="48"/>
+    </row>
+    <row r="108" spans="1:22" ht="13" customHeight="1">
       <c r="A108" s="6" t="s">
         <v>15</v>
       </c>
@@ -13022,8 +13494,11 @@
         <v>261</v>
       </c>
       <c r="S108"/>
-    </row>
-    <row r="109" spans="1:19" ht="13" customHeight="1">
+      <c r="T108" s="48"/>
+      <c r="U108" s="48"/>
+      <c r="V108" s="48"/>
+    </row>
+    <row r="109" spans="1:22" ht="13" customHeight="1">
       <c r="A109" s="6" t="s">
         <v>15</v>
       </c>
@@ -13037,8 +13512,11 @@
         <v>263</v>
       </c>
       <c r="S109"/>
-    </row>
-    <row r="110" spans="1:19" ht="13" customHeight="1">
+      <c r="T109" s="47"/>
+      <c r="U109" s="47"/>
+      <c r="V109" s="49"/>
+    </row>
+    <row r="110" spans="1:22" ht="13" customHeight="1">
       <c r="A110" s="6" t="s">
         <v>15</v>
       </c>
@@ -13053,8 +13531,11 @@
         <v>265</v>
       </c>
       <c r="S110"/>
-    </row>
-    <row r="111" spans="1:19" ht="13" customHeight="1">
+      <c r="T110" s="48"/>
+      <c r="U110" s="48"/>
+      <c r="V110" s="48"/>
+    </row>
+    <row r="111" spans="1:22" ht="13" customHeight="1">
       <c r="A111" s="6" t="s">
         <v>195</v>
       </c>
@@ -13074,8 +13555,11 @@
         <v>2181</v>
       </c>
       <c r="S111"/>
-    </row>
-    <row r="112" spans="1:19" ht="13" customHeight="1">
+      <c r="T111" s="48"/>
+      <c r="U111" s="48"/>
+      <c r="V111" s="48"/>
+    </row>
+    <row r="112" spans="1:22" ht="13" customHeight="1">
       <c r="A112" s="6" t="s">
         <v>118</v>
       </c>
@@ -13095,8 +13579,11 @@
         <v>2833</v>
       </c>
       <c r="S112"/>
-    </row>
-    <row r="113" spans="1:19" ht="13" customHeight="1">
+      <c r="T112" s="7"/>
+      <c r="U112" s="7"/>
+      <c r="V112" s="7"/>
+    </row>
+    <row r="113" spans="1:22" ht="13" customHeight="1">
       <c r="A113" s="6" t="s">
         <v>157</v>
       </c>
@@ -13137,8 +13624,11 @@
         <v>2183</v>
       </c>
       <c r="S113"/>
-    </row>
-    <row r="114" spans="1:19" ht="13" customHeight="1">
+      <c r="T113" s="7"/>
+      <c r="U113" s="7"/>
+      <c r="V113" s="7"/>
+    </row>
+    <row r="114" spans="1:22" ht="13" customHeight="1">
       <c r="A114" s="6" t="s">
         <v>39</v>
       </c>
@@ -13158,8 +13648,11 @@
         <v>2831</v>
       </c>
       <c r="S114"/>
-    </row>
-    <row r="115" spans="1:19" ht="13" customHeight="1">
+      <c r="T114" s="7"/>
+      <c r="U114" s="7"/>
+      <c r="V114" s="7"/>
+    </row>
+    <row r="115" spans="1:22" ht="13" customHeight="1">
       <c r="A115" s="6" t="s">
         <v>118</v>
       </c>
@@ -13179,8 +13672,11 @@
         <v>2184</v>
       </c>
       <c r="S115"/>
-    </row>
-    <row r="116" spans="1:19" ht="13" customHeight="1">
+      <c r="T115" s="7"/>
+      <c r="U115" s="7"/>
+      <c r="V115" s="7"/>
+    </row>
+    <row r="116" spans="1:22" ht="13" customHeight="1">
       <c r="A116" s="6" t="s">
         <v>39</v>
       </c>
@@ -13200,8 +13696,11 @@
         <v>2185</v>
       </c>
       <c r="S116"/>
-    </row>
-    <row r="117" spans="1:19" ht="13" customHeight="1">
+      <c r="T116" s="7"/>
+      <c r="U116" s="7"/>
+      <c r="V116" s="7"/>
+    </row>
+    <row r="117" spans="1:22" ht="13" customHeight="1">
       <c r="A117" s="6" t="s">
         <v>157</v>
       </c>
@@ -13242,8 +13741,11 @@
         <v>2183</v>
       </c>
       <c r="S117"/>
-    </row>
-    <row r="118" spans="1:19" ht="13" customHeight="1">
+      <c r="T117" s="7"/>
+      <c r="U117" s="7"/>
+      <c r="V117" s="7"/>
+    </row>
+    <row r="118" spans="1:22" ht="13" customHeight="1">
       <c r="A118" s="6" t="s">
         <v>118</v>
       </c>
@@ -13263,8 +13765,11 @@
         <v>2187</v>
       </c>
       <c r="S118"/>
-    </row>
-    <row r="119" spans="1:19" ht="13" customHeight="1">
+      <c r="T118" s="7"/>
+      <c r="U118" s="7"/>
+      <c r="V118" s="7"/>
+    </row>
+    <row r="119" spans="1:22" ht="13" customHeight="1">
       <c r="A119" s="6" t="s">
         <v>39</v>
       </c>
@@ -13284,8 +13789,11 @@
         <v>2188</v>
       </c>
       <c r="S119"/>
-    </row>
-    <row r="120" spans="1:19" ht="13" customHeight="1">
+      <c r="T119" s="7"/>
+      <c r="U119" s="7"/>
+      <c r="V119" s="7"/>
+    </row>
+    <row r="120" spans="1:22" ht="13" customHeight="1">
       <c r="A120" s="6" t="s">
         <v>157</v>
       </c>
@@ -13326,8 +13834,11 @@
         <v>2183</v>
       </c>
       <c r="S120"/>
-    </row>
-    <row r="121" spans="1:19" ht="13" customHeight="1">
+      <c r="T120" s="7"/>
+      <c r="U120" s="7"/>
+      <c r="V120" s="7"/>
+    </row>
+    <row r="121" spans="1:22" ht="13" customHeight="1">
       <c r="A121" s="6" t="s">
         <v>15</v>
       </c>
@@ -13339,8 +13850,11 @@
       </c>
       <c r="M121" s="4"/>
       <c r="S121"/>
-    </row>
-    <row r="122" spans="1:19" ht="13" customHeight="1">
+      <c r="T121" s="7"/>
+      <c r="U121" s="7"/>
+      <c r="V121" s="7"/>
+    </row>
+    <row r="122" spans="1:22" ht="13" customHeight="1">
       <c r="A122" s="6" t="s">
         <v>15</v>
       </c>
@@ -13351,8 +13865,11 @@
         <v>296</v>
       </c>
       <c r="S122"/>
-    </row>
-    <row r="123" spans="1:19" ht="13" customHeight="1">
+      <c r="T122" s="7"/>
+      <c r="U122" s="7"/>
+      <c r="V122" s="7"/>
+    </row>
+    <row r="123" spans="1:22" ht="13" customHeight="1">
       <c r="A123" s="6" t="s">
         <v>15</v>
       </c>
@@ -13363,8 +13880,11 @@
         <v>298</v>
       </c>
       <c r="S123"/>
-    </row>
-    <row r="124" spans="1:19" ht="13" customHeight="1">
+      <c r="T123" s="7"/>
+      <c r="U123" s="7"/>
+      <c r="V123" s="7"/>
+    </row>
+    <row r="124" spans="1:22" ht="13" customHeight="1">
       <c r="A124" s="6" t="s">
         <v>22</v>
       </c>
@@ -13381,8 +13901,11 @@
         <v>2688</v>
       </c>
       <c r="S124"/>
-    </row>
-    <row r="125" spans="1:19" ht="13" customHeight="1">
+      <c r="T124" s="7"/>
+      <c r="U124" s="7"/>
+      <c r="V124" s="7"/>
+    </row>
+    <row r="125" spans="1:22" ht="13" customHeight="1">
       <c r="A125" s="6" t="s">
         <v>15</v>
       </c>
@@ -13393,8 +13916,11 @@
         <v>303</v>
       </c>
       <c r="S125"/>
-    </row>
-    <row r="126" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T125" s="7"/>
+      <c r="U125" s="7"/>
+      <c r="V125" s="7"/>
+    </row>
+    <row r="126" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A126" s="41" t="s">
         <v>195</v>
       </c>
@@ -13414,8 +13940,11 @@
         <v>2190</v>
       </c>
       <c r="S126" s="42"/>
-    </row>
-    <row r="127" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T126" s="7"/>
+      <c r="U126" s="7"/>
+      <c r="V126" s="7"/>
+    </row>
+    <row r="127" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A127" s="41" t="s">
         <v>306</v>
       </c>
@@ -13435,8 +13964,11 @@
         <v>2789</v>
       </c>
       <c r="S127" s="42"/>
-    </row>
-    <row r="128" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T127" s="7"/>
+      <c r="U127" s="7"/>
+      <c r="V127" s="7"/>
+    </row>
+    <row r="128" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A128" s="41" t="s">
         <v>50</v>
       </c>
@@ -13471,8 +14003,11 @@
         <v>2697</v>
       </c>
       <c r="S128" s="42"/>
-    </row>
-    <row r="129" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T128" s="7"/>
+      <c r="U128" s="7"/>
+      <c r="V128" s="7"/>
+    </row>
+    <row r="129" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A129" s="41" t="s">
         <v>50</v>
       </c>
@@ -13507,8 +14042,11 @@
         <v>2697</v>
       </c>
       <c r="S129" s="42"/>
-    </row>
-    <row r="130" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T129" s="7"/>
+      <c r="U129" s="7"/>
+      <c r="V129" s="7"/>
+    </row>
+    <row r="130" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A130" s="41" t="s">
         <v>118</v>
       </c>
@@ -13528,8 +14066,11 @@
         <v>2194</v>
       </c>
       <c r="S130" s="42"/>
-    </row>
-    <row r="131" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T130" s="7"/>
+      <c r="U130" s="7"/>
+      <c r="V130" s="7"/>
+    </row>
+    <row r="131" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A131" s="41" t="s">
         <v>39</v>
       </c>
@@ -13549,8 +14090,11 @@
         <v>2195</v>
       </c>
       <c r="S131" s="42"/>
-    </row>
-    <row r="132" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T131" s="7"/>
+      <c r="U131" s="7"/>
+      <c r="V131" s="7"/>
+    </row>
+    <row r="132" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A132" s="41" t="s">
         <v>22</v>
       </c>
@@ -13567,8 +14111,11 @@
         <v>2944</v>
       </c>
       <c r="S132" s="42"/>
-    </row>
-    <row r="133" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T132" s="7"/>
+      <c r="U132" s="7"/>
+      <c r="V132" s="7"/>
+    </row>
+    <row r="133" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A133" s="41" t="s">
         <v>1005</v>
       </c>
@@ -13585,8 +14132,11 @@
         <v>2945</v>
       </c>
       <c r="S133" s="42"/>
-    </row>
-    <row r="134" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T133" s="7"/>
+      <c r="U133" s="7"/>
+      <c r="V133" s="7"/>
+    </row>
+    <row r="134" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A134" s="41" t="s">
         <v>306</v>
       </c>
@@ -13606,8 +14156,11 @@
         <v>2810</v>
       </c>
       <c r="S134" s="42"/>
-    </row>
-    <row r="135" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T134" s="7"/>
+      <c r="U134" s="7"/>
+      <c r="V134" s="7"/>
+    </row>
+    <row r="135" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A135" s="41" t="s">
         <v>15</v>
       </c>
@@ -13621,8 +14174,11 @@
         <v>2806</v>
       </c>
       <c r="S135" s="42"/>
-    </row>
-    <row r="136" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T135" s="7"/>
+      <c r="U135" s="7"/>
+      <c r="V135" s="7"/>
+    </row>
+    <row r="136" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A136" s="41" t="s">
         <v>50</v>
       </c>
@@ -13651,8 +14207,11 @@
         <v>2946</v>
       </c>
       <c r="S136" s="42"/>
-    </row>
-    <row r="137" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T136" s="7"/>
+      <c r="U136" s="7"/>
+      <c r="V136" s="7"/>
+    </row>
+    <row r="137" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A137" s="41" t="s">
         <v>1117</v>
       </c>
@@ -13661,8 +14220,11 @@
       </c>
       <c r="Q137" s="46"/>
       <c r="S137" s="42"/>
-    </row>
-    <row r="138" spans="1:19" s="41" customFormat="1" ht="13" customHeight="1">
+      <c r="T137" s="7"/>
+      <c r="U137" s="7"/>
+      <c r="V137" s="7"/>
+    </row>
+    <row r="138" spans="1:22" s="41" customFormat="1" ht="13" customHeight="1">
       <c r="A138" s="41" t="s">
         <v>15</v>
       </c>
@@ -13677,8 +14239,11 @@
       </c>
       <c r="Q138" s="46"/>
       <c r="S138" s="42"/>
-    </row>
-    <row r="139" spans="1:19" ht="13" customHeight="1">
+      <c r="T138" s="7"/>
+      <c r="U138" s="7"/>
+      <c r="V138" s="7"/>
+    </row>
+    <row r="139" spans="1:22" ht="13" customHeight="1">
       <c r="A139" s="6" t="s">
         <v>15</v>
       </c>
@@ -13692,8 +14257,11 @@
         <v>2819</v>
       </c>
       <c r="S139"/>
-    </row>
-    <row r="140" spans="1:19" ht="13" customHeight="1">
+      <c r="T139" s="7"/>
+      <c r="U139" s="7"/>
+      <c r="V139" s="7"/>
+    </row>
+    <row r="140" spans="1:22" ht="13" customHeight="1">
       <c r="A140" s="6" t="s">
         <v>15</v>
       </c>
@@ -13707,8 +14275,11 @@
         <v>2816</v>
       </c>
       <c r="S140"/>
-    </row>
-    <row r="141" spans="1:19" ht="13" customHeight="1">
+      <c r="T140" s="7"/>
+      <c r="U140" s="7"/>
+      <c r="V140" s="7"/>
+    </row>
+    <row r="141" spans="1:22" ht="13" customHeight="1">
       <c r="A141" s="6" t="s">
         <v>15</v>
       </c>
@@ -13719,8 +14290,11 @@
         <v>318</v>
       </c>
       <c r="S141"/>
-    </row>
-    <row r="142" spans="1:19" ht="13" customHeight="1">
+      <c r="T141" s="7"/>
+      <c r="U141" s="7"/>
+      <c r="V141" s="7"/>
+    </row>
+    <row r="142" spans="1:22" ht="13" customHeight="1">
       <c r="A142" s="6" t="s">
         <v>15</v>
       </c>
@@ -13734,8 +14308,11 @@
         <v>2820</v>
       </c>
       <c r="S142"/>
-    </row>
-    <row r="143" spans="1:19" ht="13" customHeight="1">
+      <c r="T142" s="7"/>
+      <c r="U142" s="7"/>
+      <c r="V142" s="7"/>
+    </row>
+    <row r="143" spans="1:22" ht="13" customHeight="1">
       <c r="A143" s="6" t="s">
         <v>15</v>
       </c>
@@ -13749,8 +14326,11 @@
         <v>2817</v>
       </c>
       <c r="S143"/>
-    </row>
-    <row r="144" spans="1:19" ht="13" customHeight="1">
+      <c r="T143" s="7"/>
+      <c r="U143" s="7"/>
+      <c r="V143" s="7"/>
+    </row>
+    <row r="144" spans="1:22" ht="13" customHeight="1">
       <c r="A144" s="6" t="s">
         <v>15</v>
       </c>
@@ -13761,8 +14341,11 @@
         <v>322</v>
       </c>
       <c r="S144"/>
-    </row>
-    <row r="145" spans="1:19" ht="13" customHeight="1">
+      <c r="T144" s="7"/>
+      <c r="U144" s="7"/>
+      <c r="V144" s="7"/>
+    </row>
+    <row r="145" spans="1:22" ht="13" customHeight="1">
       <c r="A145" s="6" t="s">
         <v>15</v>
       </c>
@@ -13773,8 +14356,11 @@
         <v>2821</v>
       </c>
       <c r="S145"/>
-    </row>
-    <row r="146" spans="1:19" ht="13" customHeight="1">
+      <c r="T145" s="7"/>
+      <c r="U145" s="7"/>
+      <c r="V145" s="7"/>
+    </row>
+    <row r="146" spans="1:22" ht="13" customHeight="1">
       <c r="A146" s="6" t="s">
         <v>15</v>
       </c>
@@ -13785,8 +14371,11 @@
         <v>2822</v>
       </c>
       <c r="S146"/>
-    </row>
-    <row r="147" spans="1:19" ht="13" customHeight="1">
+      <c r="T146" s="7"/>
+      <c r="U146" s="7"/>
+      <c r="V146" s="7"/>
+    </row>
+    <row r="147" spans="1:22" ht="13" customHeight="1">
       <c r="A147" s="6" t="s">
         <v>15</v>
       </c>
@@ -13797,8 +14386,11 @@
         <v>2823</v>
       </c>
       <c r="S147"/>
-    </row>
-    <row r="148" spans="1:19" ht="13" customHeight="1">
+      <c r="T147" s="7"/>
+      <c r="U147" s="7"/>
+      <c r="V147" s="7"/>
+    </row>
+    <row r="148" spans="1:22" ht="13" customHeight="1">
       <c r="A148" s="6" t="s">
         <v>15</v>
       </c>
@@ -13809,8 +14401,11 @@
         <v>2824</v>
       </c>
       <c r="S148"/>
-    </row>
-    <row r="149" spans="1:19" ht="13" customHeight="1">
+      <c r="T148" s="7"/>
+      <c r="U148" s="7"/>
+      <c r="V148" s="7"/>
+    </row>
+    <row r="149" spans="1:22" ht="13" customHeight="1">
       <c r="A149" s="6" t="s">
         <v>15</v>
       </c>
@@ -13821,8 +14416,11 @@
         <v>328</v>
       </c>
       <c r="S149"/>
-    </row>
-    <row r="150" spans="1:19" ht="13" customHeight="1">
+      <c r="T149" s="7"/>
+      <c r="U149" s="7"/>
+      <c r="V149" s="7"/>
+    </row>
+    <row r="150" spans="1:22" ht="13" customHeight="1">
       <c r="A150" s="6" t="s">
         <v>15</v>
       </c>
@@ -13833,8 +14431,11 @@
         <v>330</v>
       </c>
       <c r="S150"/>
-    </row>
-    <row r="151" spans="1:19" ht="13" customHeight="1">
+      <c r="T150" s="7"/>
+      <c r="U150" s="7"/>
+      <c r="V150" s="7"/>
+    </row>
+    <row r="151" spans="1:22" ht="13" customHeight="1">
       <c r="A151" s="6" t="s">
         <v>15</v>
       </c>
@@ -13845,8 +14446,11 @@
         <v>332</v>
       </c>
       <c r="S151"/>
-    </row>
-    <row r="152" spans="1:19" ht="13" customHeight="1">
+      <c r="T151" s="7"/>
+      <c r="U151" s="7"/>
+      <c r="V151" s="7"/>
+    </row>
+    <row r="152" spans="1:22" ht="13" customHeight="1">
       <c r="A152" s="6" t="s">
         <v>15</v>
       </c>
@@ -13857,8 +14461,11 @@
         <v>334</v>
       </c>
       <c r="S152"/>
-    </row>
-    <row r="153" spans="1:19" ht="13" customHeight="1">
+      <c r="T152" s="7"/>
+      <c r="U152" s="7"/>
+      <c r="V152" s="7"/>
+    </row>
+    <row r="153" spans="1:22" ht="13" customHeight="1">
       <c r="A153" s="6" t="s">
         <v>15</v>
       </c>
@@ -13869,8 +14476,11 @@
         <v>336</v>
       </c>
       <c r="S153"/>
-    </row>
-    <row r="154" spans="1:19" ht="13" customHeight="1">
+      <c r="T153" s="7"/>
+      <c r="U153" s="7"/>
+      <c r="V153" s="7"/>
+    </row>
+    <row r="154" spans="1:22" ht="13" customHeight="1">
       <c r="A154" s="6" t="s">
         <v>15</v>
       </c>
@@ -13881,8 +14491,11 @@
         <v>338</v>
       </c>
       <c r="S154"/>
-    </row>
-    <row r="155" spans="1:19" ht="13" customHeight="1">
+      <c r="T154" s="7"/>
+      <c r="U154" s="7"/>
+      <c r="V154" s="7"/>
+    </row>
+    <row r="155" spans="1:22" ht="13" customHeight="1">
       <c r="A155" s="6" t="s">
         <v>15</v>
       </c>
@@ -13893,8 +14506,11 @@
         <v>340</v>
       </c>
       <c r="S155"/>
-    </row>
-    <row r="156" spans="1:19" ht="13" customHeight="1">
+      <c r="T155" s="7"/>
+      <c r="U155" s="7"/>
+      <c r="V155" s="7"/>
+    </row>
+    <row r="156" spans="1:22" ht="13" customHeight="1">
       <c r="A156" s="6" t="s">
         <v>15</v>
       </c>
@@ -13905,8 +14521,11 @@
         <v>342</v>
       </c>
       <c r="S156"/>
-    </row>
-    <row r="157" spans="1:19" ht="13" customHeight="1">
+      <c r="T156" s="7"/>
+      <c r="U156" s="7"/>
+      <c r="V156" s="7"/>
+    </row>
+    <row r="157" spans="1:22" ht="13" customHeight="1">
       <c r="A157" s="6" t="s">
         <v>15</v>
       </c>
@@ -13917,8 +14536,11 @@
         <v>344</v>
       </c>
       <c r="S157"/>
-    </row>
-    <row r="158" spans="1:19" ht="13" customHeight="1">
+      <c r="T157" s="7"/>
+      <c r="U157" s="7"/>
+      <c r="V157" s="7"/>
+    </row>
+    <row r="158" spans="1:22" ht="13" customHeight="1">
       <c r="A158" s="6" t="s">
         <v>15</v>
       </c>
@@ -13929,8 +14551,11 @@
         <v>2825</v>
       </c>
       <c r="S158"/>
-    </row>
-    <row r="159" spans="1:19" ht="13" customHeight="1">
+      <c r="T158" s="7"/>
+      <c r="U158" s="7"/>
+      <c r="V158" s="7"/>
+    </row>
+    <row r="159" spans="1:22" ht="13" customHeight="1">
       <c r="A159" s="6" t="s">
         <v>15</v>
       </c>
@@ -13941,8 +14566,11 @@
         <v>2917</v>
       </c>
       <c r="S159"/>
-    </row>
-    <row r="160" spans="1:19" ht="13" customHeight="1">
+      <c r="T159" s="7"/>
+      <c r="U159" s="7"/>
+      <c r="V159" s="7"/>
+    </row>
+    <row r="160" spans="1:22" ht="13" customHeight="1">
       <c r="A160" s="6" t="s">
         <v>15</v>
       </c>
@@ -13953,8 +14581,11 @@
         <v>2919</v>
       </c>
       <c r="S160"/>
-    </row>
-    <row r="161" spans="1:19" ht="13" customHeight="1">
+      <c r="T160" s="7"/>
+      <c r="U160" s="7"/>
+      <c r="V160" s="7"/>
+    </row>
+    <row r="161" spans="1:22" ht="13" customHeight="1">
       <c r="A161" s="6" t="s">
         <v>15</v>
       </c>
@@ -13965,8 +14596,11 @@
         <v>2826</v>
       </c>
       <c r="S161"/>
-    </row>
-    <row r="162" spans="1:19" ht="13" customHeight="1">
+      <c r="T161" s="7"/>
+      <c r="U161" s="7"/>
+      <c r="V161" s="7"/>
+    </row>
+    <row r="162" spans="1:22" ht="13" customHeight="1">
       <c r="A162" s="6" t="s">
         <v>347</v>
       </c>
@@ -13986,8 +14620,11 @@
         <v>2196</v>
       </c>
       <c r="S162"/>
-    </row>
-    <row r="163" spans="1:19" ht="13" customHeight="1">
+      <c r="T162" s="7"/>
+      <c r="U162" s="7"/>
+      <c r="V162" s="7"/>
+    </row>
+    <row r="163" spans="1:22" ht="13" customHeight="1">
       <c r="A163" s="6" t="s">
         <v>15</v>
       </c>
@@ -14001,8 +14638,11 @@
         <v>352</v>
       </c>
       <c r="S163"/>
-    </row>
-    <row r="164" spans="1:19" ht="13" customHeight="1">
+      <c r="T163" s="7"/>
+      <c r="U163" s="7"/>
+      <c r="V163" s="7"/>
+    </row>
+    <row r="164" spans="1:22" ht="13" customHeight="1">
       <c r="A164" s="6" t="s">
         <v>18</v>
       </c>
@@ -14016,8 +14656,11 @@
         <v>354</v>
       </c>
       <c r="S164"/>
-    </row>
-    <row r="165" spans="1:19" ht="13" customHeight="1">
+      <c r="T164" s="7"/>
+      <c r="U164" s="7"/>
+      <c r="V164" s="7"/>
+    </row>
+    <row r="165" spans="1:22" ht="13" customHeight="1">
       <c r="A165" s="6" t="s">
         <v>22</v>
       </c>
@@ -14031,8 +14674,11 @@
         <v>2197</v>
       </c>
       <c r="S165"/>
-    </row>
-    <row r="166" spans="1:19" ht="13" customHeight="1">
+      <c r="T165" s="7"/>
+      <c r="U165" s="7"/>
+      <c r="V165" s="7"/>
+    </row>
+    <row r="166" spans="1:22" ht="13" customHeight="1">
       <c r="A166" s="6" t="s">
         <v>22</v>
       </c>
@@ -14049,8 +14695,11 @@
         <v>2198</v>
       </c>
       <c r="S166"/>
-    </row>
-    <row r="167" spans="1:19" ht="13" customHeight="1">
+      <c r="T166" s="7"/>
+      <c r="U166" s="7"/>
+      <c r="V166" s="7"/>
+    </row>
+    <row r="167" spans="1:22" ht="13" customHeight="1">
       <c r="A167" s="6" t="s">
         <v>50</v>
       </c>
@@ -14082,8 +14731,11 @@
         <v>2908</v>
       </c>
       <c r="S167"/>
-    </row>
-    <row r="168" spans="1:19" ht="13" customHeight="1">
+      <c r="T167" s="7"/>
+      <c r="U167" s="7"/>
+      <c r="V167" s="7"/>
+    </row>
+    <row r="168" spans="1:22" ht="13" customHeight="1">
       <c r="A168" s="6" t="s">
         <v>29</v>
       </c>
@@ -14091,11 +14743,17 @@
         <v>353</v>
       </c>
       <c r="S168"/>
-    </row>
-    <row r="169" spans="1:19" ht="13" customHeight="1">
+      <c r="T168" s="7"/>
+      <c r="U168" s="7"/>
+      <c r="V168" s="7"/>
+    </row>
+    <row r="169" spans="1:22" ht="13" customHeight="1">
       <c r="S169"/>
-    </row>
-    <row r="170" spans="1:19" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="T169" s="7"/>
+      <c r="U169" s="7"/>
+      <c r="V169" s="7"/>
+    </row>
+    <row r="170" spans="1:22" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A170" s="8" t="s">
         <v>22</v>
       </c>
@@ -14119,8 +14777,11 @@
       </c>
       <c r="R170" s="6"/>
       <c r="S170"/>
-    </row>
-    <row r="171" spans="1:19" ht="13" customHeight="1">
+      <c r="T170" s="7"/>
+      <c r="U170" s="7"/>
+      <c r="V170" s="7"/>
+    </row>
+    <row r="171" spans="1:22" ht="13" customHeight="1">
       <c r="A171" s="6" t="s">
         <v>18</v>
       </c>
@@ -14131,8 +14792,11 @@
         <v>354</v>
       </c>
       <c r="S171"/>
-    </row>
-    <row r="172" spans="1:19" ht="13" customHeight="1">
+      <c r="T171" s="7"/>
+      <c r="U171" s="7"/>
+      <c r="V171" s="7"/>
+    </row>
+    <row r="172" spans="1:22" ht="13" customHeight="1">
       <c r="A172" s="6" t="s">
         <v>195</v>
       </c>
@@ -14149,8 +14813,11 @@
         <v>2890</v>
       </c>
       <c r="S172"/>
-    </row>
-    <row r="173" spans="1:19" ht="13" customHeight="1">
+      <c r="T172" s="7"/>
+      <c r="U172" s="7"/>
+      <c r="V172" s="7"/>
+    </row>
+    <row r="173" spans="1:22" ht="13" customHeight="1">
       <c r="A173" s="6" t="s">
         <v>368</v>
       </c>
@@ -14176,8 +14843,11 @@
         <v>2203</v>
       </c>
       <c r="S173"/>
-    </row>
-    <row r="174" spans="1:19" ht="13" customHeight="1">
+      <c r="T173" s="7"/>
+      <c r="U173" s="7"/>
+      <c r="V173" s="7"/>
+    </row>
+    <row r="174" spans="1:22" ht="13" customHeight="1">
       <c r="A174" s="6" t="s">
         <v>373</v>
       </c>
@@ -14197,8 +14867,11 @@
         <v>2204</v>
       </c>
       <c r="S174"/>
-    </row>
-    <row r="175" spans="1:19" ht="13" customHeight="1">
+      <c r="T174" s="7"/>
+      <c r="U174" s="7"/>
+      <c r="V174" s="7"/>
+    </row>
+    <row r="175" spans="1:22" ht="13" customHeight="1">
       <c r="A175" s="6" t="s">
         <v>118</v>
       </c>
@@ -14218,8 +14891,11 @@
         <v>2895</v>
       </c>
       <c r="S175"/>
-    </row>
-    <row r="176" spans="1:19" ht="13" customHeight="1">
+      <c r="T175" s="7"/>
+      <c r="U175" s="7"/>
+      <c r="V175" s="7"/>
+    </row>
+    <row r="176" spans="1:22" ht="13" customHeight="1">
       <c r="A176" s="6" t="s">
         <v>18</v>
       </c>
@@ -14233,8 +14909,11 @@
         <v>379</v>
       </c>
       <c r="S176"/>
-    </row>
-    <row r="177" spans="1:19" ht="13" customHeight="1">
+      <c r="T176" s="7"/>
+      <c r="U176" s="7"/>
+      <c r="V176" s="7"/>
+    </row>
+    <row r="177" spans="1:22" ht="13" customHeight="1">
       <c r="A177" s="6" t="s">
         <v>380</v>
       </c>
@@ -14266,8 +14945,11 @@
         <v>2207</v>
       </c>
       <c r="S177"/>
-    </row>
-    <row r="178" spans="1:19" ht="13" customHeight="1">
+      <c r="T177" s="7"/>
+      <c r="U177" s="7"/>
+      <c r="V177" s="7"/>
+    </row>
+    <row r="178" spans="1:22" ht="13" customHeight="1">
       <c r="A178" s="6" t="s">
         <v>130</v>
       </c>
@@ -14284,8 +14966,11 @@
         <v>2208</v>
       </c>
       <c r="S178"/>
-    </row>
-    <row r="179" spans="1:19" ht="13" customHeight="1">
+      <c r="T178" s="7"/>
+      <c r="U178" s="7"/>
+      <c r="V178" s="7"/>
+    </row>
+    <row r="179" spans="1:22" ht="13" customHeight="1">
       <c r="A179" s="6" t="s">
         <v>29</v>
       </c>
@@ -14293,8 +14978,11 @@
         <v>378</v>
       </c>
       <c r="S179"/>
-    </row>
-    <row r="180" spans="1:19" ht="13" customHeight="1">
+      <c r="T179" s="7"/>
+      <c r="U179" s="7"/>
+      <c r="V179" s="7"/>
+    </row>
+    <row r="180" spans="1:22" ht="13" customHeight="1">
       <c r="A180" s="6" t="s">
         <v>118</v>
       </c>
@@ -14311,8 +14999,11 @@
         <v>2953</v>
       </c>
       <c r="S180"/>
-    </row>
-    <row r="181" spans="1:19" ht="13" customHeight="1">
+      <c r="T180" s="7"/>
+      <c r="U180" s="7"/>
+      <c r="V180" s="7"/>
+    </row>
+    <row r="181" spans="1:22" ht="13" customHeight="1">
       <c r="A181" s="6" t="s">
         <v>18</v>
       </c>
@@ -14326,8 +15017,11 @@
         <v>390</v>
       </c>
       <c r="S181"/>
-    </row>
-    <row r="182" spans="1:19" ht="13" customHeight="1">
+      <c r="T181" s="7"/>
+      <c r="U181" s="7"/>
+      <c r="V181" s="7"/>
+    </row>
+    <row r="182" spans="1:22" ht="13" customHeight="1">
       <c r="A182" s="6" t="s">
         <v>391</v>
       </c>
@@ -14359,8 +15053,11 @@
         <v>2207</v>
       </c>
       <c r="S182"/>
-    </row>
-    <row r="183" spans="1:19" ht="13" customHeight="1">
+      <c r="T182" s="7"/>
+      <c r="U182" s="7"/>
+      <c r="V182" s="7"/>
+    </row>
+    <row r="183" spans="1:22" ht="13" customHeight="1">
       <c r="A183" s="6" t="s">
         <v>130</v>
       </c>
@@ -14377,8 +15074,11 @@
         <v>2208</v>
       </c>
       <c r="S183"/>
-    </row>
-    <row r="184" spans="1:19" ht="13" customHeight="1">
+      <c r="T183" s="7"/>
+      <c r="U183" s="7"/>
+      <c r="V183" s="7"/>
+    </row>
+    <row r="184" spans="1:22" ht="13" customHeight="1">
       <c r="A184" s="6" t="s">
         <v>29</v>
       </c>
@@ -14386,8 +15086,11 @@
         <v>389</v>
       </c>
       <c r="S184"/>
-    </row>
-    <row r="185" spans="1:19" ht="13" customHeight="1">
+      <c r="T184" s="7"/>
+      <c r="U184" s="7"/>
+      <c r="V184" s="7"/>
+    </row>
+    <row r="185" spans="1:22" ht="13" customHeight="1">
       <c r="A185" s="6" t="s">
         <v>18</v>
       </c>
@@ -14401,8 +15104,11 @@
         <v>396</v>
       </c>
       <c r="S185"/>
-    </row>
-    <row r="186" spans="1:19" ht="13" customHeight="1">
+      <c r="T185" s="7"/>
+      <c r="U185" s="7"/>
+      <c r="V185" s="7"/>
+    </row>
+    <row r="186" spans="1:22" ht="13" customHeight="1">
       <c r="A186" s="6" t="s">
         <v>397</v>
       </c>
@@ -14434,8 +15140,11 @@
         <v>2209</v>
       </c>
       <c r="S186"/>
-    </row>
-    <row r="187" spans="1:19" ht="13" customHeight="1">
+      <c r="T186" s="7"/>
+      <c r="U186" s="7"/>
+      <c r="V186" s="7"/>
+    </row>
+    <row r="187" spans="1:22" ht="13" customHeight="1">
       <c r="A187" s="6" t="s">
         <v>130</v>
       </c>
@@ -14452,8 +15161,11 @@
         <v>2208</v>
       </c>
       <c r="S187"/>
-    </row>
-    <row r="188" spans="1:19" ht="13" customHeight="1">
+      <c r="T187" s="7"/>
+      <c r="U187" s="7"/>
+      <c r="V187" s="7"/>
+    </row>
+    <row r="188" spans="1:22" ht="13" customHeight="1">
       <c r="A188" s="6" t="s">
         <v>29</v>
       </c>
@@ -14461,8 +15173,11 @@
         <v>395</v>
       </c>
       <c r="S188"/>
-    </row>
-    <row r="189" spans="1:19" ht="13" customHeight="1">
+      <c r="T188" s="7"/>
+      <c r="U188" s="7"/>
+      <c r="V188" s="7"/>
+    </row>
+    <row r="189" spans="1:22" ht="13" customHeight="1">
       <c r="A189" s="6" t="s">
         <v>118</v>
       </c>
@@ -14482,8 +15197,11 @@
         <v>2892</v>
       </c>
       <c r="S189"/>
-    </row>
-    <row r="190" spans="1:19" ht="13" customHeight="1">
+      <c r="T189" s="7"/>
+      <c r="U189" s="7"/>
+      <c r="V189" s="7"/>
+    </row>
+    <row r="190" spans="1:22" ht="13" customHeight="1">
       <c r="A190" s="6" t="s">
         <v>18</v>
       </c>
@@ -14497,8 +15215,11 @@
         <v>405</v>
       </c>
       <c r="S190"/>
-    </row>
-    <row r="191" spans="1:19" ht="13" customHeight="1">
+      <c r="T190" s="7"/>
+      <c r="U190" s="7"/>
+      <c r="V190" s="7"/>
+    </row>
+    <row r="191" spans="1:22" ht="13" customHeight="1">
       <c r="A191" s="6" t="s">
         <v>380</v>
       </c>
@@ -14530,8 +15251,11 @@
         <v>2207</v>
       </c>
       <c r="S191"/>
-    </row>
-    <row r="192" spans="1:19" ht="13" customHeight="1">
+      <c r="T191" s="7"/>
+      <c r="U191" s="7"/>
+      <c r="V191" s="7"/>
+    </row>
+    <row r="192" spans="1:22" ht="13" customHeight="1">
       <c r="A192" s="6" t="s">
         <v>130</v>
       </c>
@@ -14548,8 +15272,11 @@
         <v>2208</v>
       </c>
       <c r="S192"/>
-    </row>
-    <row r="193" spans="1:19" ht="13" customHeight="1">
+      <c r="T192" s="7"/>
+      <c r="U192" s="7"/>
+      <c r="V192" s="7"/>
+    </row>
+    <row r="193" spans="1:22" ht="13" customHeight="1">
       <c r="A193" s="6" t="s">
         <v>29</v>
       </c>
@@ -14557,8 +15284,11 @@
         <v>404</v>
       </c>
       <c r="S193"/>
-    </row>
-    <row r="194" spans="1:19" ht="13" customHeight="1">
+      <c r="T193" s="7"/>
+      <c r="U193" s="7"/>
+      <c r="V193" s="7"/>
+    </row>
+    <row r="194" spans="1:22" ht="13" customHeight="1">
       <c r="A194" s="6" t="s">
         <v>118</v>
       </c>
@@ -14575,8 +15305,11 @@
         <v>2893</v>
       </c>
       <c r="S194"/>
-    </row>
-    <row r="195" spans="1:19" ht="13" customHeight="1">
+      <c r="T194" s="7"/>
+      <c r="U194" s="7"/>
+      <c r="V194" s="7"/>
+    </row>
+    <row r="195" spans="1:22" ht="13" customHeight="1">
       <c r="A195" s="6" t="s">
         <v>18</v>
       </c>
@@ -14590,8 +15323,11 @@
         <v>412</v>
       </c>
       <c r="S195"/>
-    </row>
-    <row r="196" spans="1:19" ht="13" customHeight="1">
+      <c r="T195" s="7"/>
+      <c r="U195" s="7"/>
+      <c r="V195" s="7"/>
+    </row>
+    <row r="196" spans="1:22" ht="13" customHeight="1">
       <c r="A196" s="6" t="s">
         <v>391</v>
       </c>
@@ -14623,8 +15359,11 @@
         <v>2207</v>
       </c>
       <c r="S196"/>
-    </row>
-    <row r="197" spans="1:19" ht="13" customHeight="1">
+      <c r="T196" s="7"/>
+      <c r="U196" s="7"/>
+      <c r="V196" s="7"/>
+    </row>
+    <row r="197" spans="1:22" ht="13" customHeight="1">
       <c r="A197" s="6" t="s">
         <v>130</v>
       </c>
@@ -14641,8 +15380,11 @@
         <v>2208</v>
       </c>
       <c r="S197"/>
-    </row>
-    <row r="198" spans="1:19" ht="13" customHeight="1">
+      <c r="T197" s="7"/>
+      <c r="U197" s="7"/>
+      <c r="V197" s="7"/>
+    </row>
+    <row r="198" spans="1:22" ht="13" customHeight="1">
       <c r="A198" s="6" t="s">
         <v>29</v>
       </c>
@@ -14650,8 +15392,11 @@
         <v>411</v>
       </c>
       <c r="S198"/>
-    </row>
-    <row r="199" spans="1:19" s="4" customFormat="1" ht="13" customHeight="1">
+      <c r="T198" s="7"/>
+      <c r="U198" s="7"/>
+      <c r="V198" s="7"/>
+    </row>
+    <row r="199" spans="1:22" s="4" customFormat="1" ht="13" customHeight="1">
       <c r="A199" s="4" t="s">
         <v>18</v>
       </c>
@@ -14668,8 +15413,11 @@
       <c r="Q199" s="6"/>
       <c r="R199" s="6"/>
       <c r="S199"/>
-    </row>
-    <row r="200" spans="1:19" s="4" customFormat="1" ht="13" customHeight="1">
+      <c r="T199" s="7"/>
+      <c r="U199" s="7"/>
+      <c r="V199" s="7"/>
+    </row>
+    <row r="200" spans="1:22" s="4" customFormat="1" ht="13" customHeight="1">
       <c r="A200" s="4" t="s">
         <v>416</v>
       </c>
@@ -14701,8 +15449,11 @@
         <v>2209</v>
       </c>
       <c r="S200"/>
-    </row>
-    <row r="201" spans="1:19" s="4" customFormat="1" ht="13" customHeight="1">
+      <c r="T200" s="7"/>
+      <c r="U200" s="7"/>
+      <c r="V200" s="7"/>
+    </row>
+    <row r="201" spans="1:22" s="4" customFormat="1" ht="13" customHeight="1">
       <c r="A201" s="4" t="s">
         <v>130</v>
       </c>
@@ -14721,8 +15472,11 @@
       <c r="Q201" s="6"/>
       <c r="R201" s="6"/>
       <c r="S201"/>
-    </row>
-    <row r="202" spans="1:19" s="4" customFormat="1" ht="13" customHeight="1">
+      <c r="T201" s="7"/>
+      <c r="U201" s="7"/>
+      <c r="V201" s="7"/>
+    </row>
+    <row r="202" spans="1:22" s="4" customFormat="1" ht="13" customHeight="1">
       <c r="A202" s="4" t="s">
         <v>29</v>
       </c>
@@ -14733,8 +15487,11 @@
       <c r="Q202" s="6"/>
       <c r="R202" s="6"/>
       <c r="S202"/>
-    </row>
-    <row r="203" spans="1:19" ht="13" customHeight="1">
+      <c r="T202" s="7"/>
+      <c r="U202" s="7"/>
+      <c r="V202" s="7"/>
+    </row>
+    <row r="203" spans="1:22" ht="13" customHeight="1">
       <c r="A203" s="6" t="s">
         <v>118</v>
       </c>
@@ -14754,8 +15511,11 @@
         <v>2896</v>
       </c>
       <c r="S203"/>
-    </row>
-    <row r="204" spans="1:19" ht="13" customHeight="1">
+      <c r="T203" s="7"/>
+      <c r="U203" s="7"/>
+      <c r="V203" s="7"/>
+    </row>
+    <row r="204" spans="1:22" ht="13" customHeight="1">
       <c r="A204" s="6" t="s">
         <v>118</v>
       </c>
@@ -14775,8 +15535,11 @@
         <v>2897</v>
       </c>
       <c r="S204"/>
-    </row>
-    <row r="205" spans="1:19" ht="13" customHeight="1">
+      <c r="T204" s="7"/>
+      <c r="U204" s="7"/>
+      <c r="V204" s="7"/>
+    </row>
+    <row r="205" spans="1:22" ht="13" customHeight="1">
       <c r="A205" s="6" t="s">
         <v>118</v>
       </c>
@@ -14796,8 +15559,11 @@
         <v>2898</v>
       </c>
       <c r="S205"/>
-    </row>
-    <row r="206" spans="1:19" ht="13" customHeight="1">
+      <c r="T205" s="7"/>
+      <c r="U205" s="7"/>
+      <c r="V205" s="7"/>
+    </row>
+    <row r="206" spans="1:22" ht="13" customHeight="1">
       <c r="A206" s="6" t="s">
         <v>118</v>
       </c>
@@ -14817,11 +15583,17 @@
         <v>2894</v>
       </c>
       <c r="S206"/>
-    </row>
-    <row r="207" spans="1:19" ht="13" customHeight="1">
+      <c r="T206" s="7"/>
+      <c r="U206" s="7"/>
+      <c r="V206" s="7"/>
+    </row>
+    <row r="207" spans="1:22" ht="13" customHeight="1">
       <c r="S207"/>
-    </row>
-    <row r="208" spans="1:19" ht="13" customHeight="1">
+      <c r="T207" s="7"/>
+      <c r="U207" s="7"/>
+      <c r="V207" s="7"/>
+    </row>
+    <row r="208" spans="1:22" ht="13" customHeight="1">
       <c r="A208" s="6" t="s">
         <v>18</v>
       </c>
@@ -14835,8 +15607,11 @@
         <v>372</v>
       </c>
       <c r="S208"/>
-    </row>
-    <row r="209" spans="1:19" ht="13" customHeight="1">
+      <c r="T208" s="7"/>
+      <c r="U208" s="7"/>
+      <c r="V208" s="7"/>
+    </row>
+    <row r="209" spans="1:22" ht="13" customHeight="1">
       <c r="A209" s="6" t="s">
         <v>431</v>
       </c>
@@ -14868,8 +15643,11 @@
         <v>2213</v>
       </c>
       <c r="S209"/>
-    </row>
-    <row r="210" spans="1:19" ht="13" customHeight="1">
+      <c r="T209" s="7"/>
+      <c r="U209" s="7"/>
+      <c r="V209" s="7"/>
+    </row>
+    <row r="210" spans="1:22" ht="13" customHeight="1">
       <c r="A210" s="6" t="s">
         <v>15</v>
       </c>
@@ -14880,8 +15658,11 @@
         <v>438</v>
       </c>
       <c r="S210"/>
-    </row>
-    <row r="211" spans="1:19" ht="13" customHeight="1">
+      <c r="T210" s="7"/>
+      <c r="U210" s="7"/>
+      <c r="V210" s="7"/>
+    </row>
+    <row r="211" spans="1:22" ht="13" customHeight="1">
       <c r="A211" s="6" t="s">
         <v>22</v>
       </c>
@@ -14900,8 +15681,11 @@
       <c r="S211" s="13" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="212" spans="1:19" ht="13" customHeight="1">
+      <c r="T211" s="7"/>
+      <c r="U211" s="7"/>
+      <c r="V211" s="7"/>
+    </row>
+    <row r="212" spans="1:22" ht="13" customHeight="1">
       <c r="A212" s="6" t="s">
         <v>29</v>
       </c>
@@ -14909,8 +15693,11 @@
         <v>430</v>
       </c>
       <c r="S212"/>
-    </row>
-    <row r="213" spans="1:19" ht="13" customHeight="1">
+      <c r="T212" s="7"/>
+      <c r="U212" s="7"/>
+      <c r="V212" s="7"/>
+    </row>
+    <row r="213" spans="1:22" ht="13" customHeight="1">
       <c r="A213" s="6" t="s">
         <v>118</v>
       </c>
@@ -14930,8 +15717,11 @@
         <v>2722</v>
       </c>
       <c r="S213"/>
-    </row>
-    <row r="214" spans="1:19" ht="13" customHeight="1">
+      <c r="T213" s="7"/>
+      <c r="U213" s="7"/>
+      <c r="V213" s="7"/>
+    </row>
+    <row r="214" spans="1:22" ht="13" customHeight="1">
       <c r="A214" s="6" t="s">
         <v>195</v>
       </c>
@@ -14951,8 +15741,11 @@
         <v>2214</v>
       </c>
       <c r="S214"/>
-    </row>
-    <row r="215" spans="1:19" ht="13" customHeight="1">
+      <c r="T214" s="7"/>
+      <c r="U214" s="7"/>
+      <c r="V214" s="7"/>
+    </row>
+    <row r="215" spans="1:22" ht="13" customHeight="1">
       <c r="A215" s="6" t="s">
         <v>195</v>
       </c>
@@ -14972,8 +15765,11 @@
         <v>2215</v>
       </c>
       <c r="S215"/>
-    </row>
-    <row r="216" spans="1:19" ht="13" customHeight="1">
+      <c r="T215" s="7"/>
+      <c r="U215" s="7"/>
+      <c r="V215" s="7"/>
+    </row>
+    <row r="216" spans="1:22" ht="13" customHeight="1">
       <c r="A216" s="6" t="s">
         <v>50</v>
       </c>
@@ -15008,8 +15804,11 @@
         <v>2698</v>
       </c>
       <c r="S216"/>
-    </row>
-    <row r="217" spans="1:19" ht="13" customHeight="1">
+      <c r="T216" s="7"/>
+      <c r="U216" s="7"/>
+      <c r="V216" s="7"/>
+    </row>
+    <row r="217" spans="1:22" ht="13" customHeight="1">
       <c r="A217" s="6" t="s">
         <v>50</v>
       </c>
@@ -15044,8 +15843,11 @@
         <v>2699</v>
       </c>
       <c r="S217"/>
-    </row>
-    <row r="218" spans="1:19" ht="13" customHeight="1">
+      <c r="T217" s="7"/>
+      <c r="U217" s="7"/>
+      <c r="V217" s="7"/>
+    </row>
+    <row r="218" spans="1:22" ht="13" customHeight="1">
       <c r="A218" s="6" t="s">
         <v>18</v>
       </c>
@@ -15059,8 +15861,11 @@
         <v>372</v>
       </c>
       <c r="S218"/>
-    </row>
-    <row r="219" spans="1:19" ht="13" customHeight="1">
+      <c r="T218" s="7"/>
+      <c r="U218" s="7"/>
+      <c r="V218" s="7"/>
+    </row>
+    <row r="219" spans="1:22" ht="13" customHeight="1">
       <c r="A219" s="6" t="s">
         <v>431</v>
       </c>
@@ -15092,8 +15897,11 @@
         <v>2213</v>
       </c>
       <c r="S219"/>
-    </row>
-    <row r="220" spans="1:19" ht="13" customHeight="1">
+      <c r="T219" s="7"/>
+      <c r="U219" s="7"/>
+      <c r="V219" s="7"/>
+    </row>
+    <row r="220" spans="1:22" ht="13" customHeight="1">
       <c r="A220" s="6" t="s">
         <v>15</v>
       </c>
@@ -15104,8 +15912,11 @@
         <v>465</v>
       </c>
       <c r="S220"/>
-    </row>
-    <row r="221" spans="1:19" ht="13" customHeight="1">
+      <c r="T220" s="7"/>
+      <c r="U220" s="7"/>
+      <c r="V220" s="7"/>
+    </row>
+    <row r="221" spans="1:22" ht="13" customHeight="1">
       <c r="A221" s="6" t="s">
         <v>22</v>
       </c>
@@ -15124,8 +15935,11 @@
       <c r="S221" s="13" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="222" spans="1:19" ht="13" customHeight="1">
+      <c r="T221" s="7"/>
+      <c r="U221" s="7"/>
+      <c r="V221" s="7"/>
+    </row>
+    <row r="222" spans="1:22" ht="13" customHeight="1">
       <c r="A222" s="6" t="s">
         <v>29</v>
       </c>
@@ -15133,8 +15947,11 @@
         <v>460</v>
       </c>
       <c r="S222"/>
-    </row>
-    <row r="223" spans="1:19" ht="13" customHeight="1">
+      <c r="T222" s="7"/>
+      <c r="U222" s="7"/>
+      <c r="V222" s="7"/>
+    </row>
+    <row r="223" spans="1:22" ht="13" customHeight="1">
       <c r="A223" s="6" t="s">
         <v>118</v>
       </c>
@@ -15154,8 +15971,11 @@
         <v>2723</v>
       </c>
       <c r="S223"/>
-    </row>
-    <row r="224" spans="1:19" ht="13" customHeight="1">
+      <c r="T223" s="7"/>
+      <c r="U223" s="7"/>
+      <c r="V223" s="7"/>
+    </row>
+    <row r="224" spans="1:22" ht="13" customHeight="1">
       <c r="A224" s="6" t="s">
         <v>195</v>
       </c>
@@ -15175,8 +15995,11 @@
         <v>2219</v>
       </c>
       <c r="S224"/>
-    </row>
-    <row r="225" spans="1:19" ht="13" customHeight="1">
+      <c r="T224" s="7"/>
+      <c r="U224" s="7"/>
+      <c r="V224" s="7"/>
+    </row>
+    <row r="225" spans="1:22" ht="13" customHeight="1">
       <c r="A225" s="6" t="s">
         <v>195</v>
       </c>
@@ -15196,8 +16019,11 @@
         <v>2220</v>
       </c>
       <c r="S225"/>
-    </row>
-    <row r="226" spans="1:19" ht="13" customHeight="1">
+      <c r="T225" s="7"/>
+      <c r="U225" s="7"/>
+      <c r="V225" s="7"/>
+    </row>
+    <row r="226" spans="1:22" ht="13" customHeight="1">
       <c r="A226" s="6" t="s">
         <v>50</v>
       </c>
@@ -15232,8 +16058,11 @@
         <v>2698</v>
       </c>
       <c r="S226"/>
-    </row>
-    <row r="227" spans="1:19" ht="13" customHeight="1">
+      <c r="T226" s="7"/>
+      <c r="U226" s="7"/>
+      <c r="V226" s="7"/>
+    </row>
+    <row r="227" spans="1:22" ht="13" customHeight="1">
       <c r="A227" s="6" t="s">
         <v>50</v>
       </c>
@@ -15268,8 +16097,11 @@
         <v>2699</v>
       </c>
       <c r="S227"/>
-    </row>
-    <row r="228" spans="1:19" ht="13" customHeight="1">
+      <c r="T227" s="7"/>
+      <c r="U227" s="7"/>
+      <c r="V227" s="7"/>
+    </row>
+    <row r="228" spans="1:22" ht="13" customHeight="1">
       <c r="A228" s="6" t="s">
         <v>18</v>
       </c>
@@ -15280,8 +16112,11 @@
         <v>20</v>
       </c>
       <c r="S228"/>
-    </row>
-    <row r="229" spans="1:19" ht="13" customHeight="1">
+      <c r="T228" s="7"/>
+      <c r="U228" s="7"/>
+      <c r="V228" s="7"/>
+    </row>
+    <row r="229" spans="1:22" ht="13" customHeight="1">
       <c r="A229" s="6" t="s">
         <v>118</v>
       </c>
@@ -15304,8 +16139,11 @@
         <v>2222</v>
       </c>
       <c r="S229"/>
-    </row>
-    <row r="230" spans="1:19" ht="13" customHeight="1">
+      <c r="T229" s="7"/>
+      <c r="U229" s="7"/>
+      <c r="V229" s="7"/>
+    </row>
+    <row r="230" spans="1:22" ht="13" customHeight="1">
       <c r="A230" s="6" t="s">
         <v>22</v>
       </c>
@@ -15318,8 +16156,11 @@
       <c r="S230" s="13" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="231" spans="1:19" ht="13" customHeight="1">
+      <c r="T230" s="7"/>
+      <c r="U230" s="7"/>
+      <c r="V230" s="7"/>
+    </row>
+    <row r="231" spans="1:22" ht="13" customHeight="1">
       <c r="A231" s="6" t="s">
         <v>29</v>
       </c>
@@ -15327,8 +16168,11 @@
         <v>481</v>
       </c>
       <c r="S231"/>
-    </row>
-    <row r="232" spans="1:19" ht="13" customHeight="1">
+      <c r="T231" s="7"/>
+      <c r="U231" s="7"/>
+      <c r="V231" s="7"/>
+    </row>
+    <row r="232" spans="1:22" ht="13" customHeight="1">
       <c r="A232" s="6" t="s">
         <v>118</v>
       </c>
@@ -15345,8 +16189,11 @@
         <v>2223</v>
       </c>
       <c r="S232"/>
-    </row>
-    <row r="233" spans="1:19" ht="13" customHeight="1">
+      <c r="T232" s="7"/>
+      <c r="U232" s="7"/>
+      <c r="V232" s="7"/>
+    </row>
+    <row r="233" spans="1:22" ht="13" customHeight="1">
       <c r="A233" s="6" t="s">
         <v>118</v>
       </c>
@@ -15366,8 +16213,11 @@
         <v>2902</v>
       </c>
       <c r="S233"/>
-    </row>
-    <row r="234" spans="1:19" ht="13" customHeight="1">
+      <c r="T233" s="7"/>
+      <c r="U233" s="7"/>
+      <c r="V233" s="7"/>
+    </row>
+    <row r="234" spans="1:22" ht="13" customHeight="1">
       <c r="A234" s="6" t="s">
         <v>118</v>
       </c>
@@ -15384,8 +16234,11 @@
         <v>2903</v>
       </c>
       <c r="S234"/>
-    </row>
-    <row r="235" spans="1:19" ht="13" customHeight="1">
+      <c r="T234" s="7"/>
+      <c r="U234" s="7"/>
+      <c r="V234" s="7"/>
+    </row>
+    <row r="235" spans="1:22" ht="13" customHeight="1">
       <c r="A235" s="6" t="s">
         <v>18</v>
       </c>
@@ -15399,8 +16252,11 @@
         <v>494</v>
       </c>
       <c r="S235"/>
-    </row>
-    <row r="236" spans="1:19" ht="13" customHeight="1">
+      <c r="T235" s="7"/>
+      <c r="U235" s="7"/>
+      <c r="V235" s="7"/>
+    </row>
+    <row r="236" spans="1:22" ht="13" customHeight="1">
       <c r="A236" s="6" t="s">
         <v>495</v>
       </c>
@@ -15432,8 +16288,11 @@
         <v>2213</v>
       </c>
       <c r="S236"/>
-    </row>
-    <row r="237" spans="1:19" ht="13" customHeight="1">
+      <c r="T236" s="7"/>
+      <c r="U236" s="7"/>
+      <c r="V236" s="7"/>
+    </row>
+    <row r="237" spans="1:22" ht="13" customHeight="1">
       <c r="A237" s="6" t="s">
         <v>22</v>
       </c>
@@ -15446,8 +16305,11 @@
       <c r="S237" s="13" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="238" spans="1:19" ht="13" customHeight="1">
+      <c r="T237" s="7"/>
+      <c r="U237" s="7"/>
+      <c r="V237" s="7"/>
+    </row>
+    <row r="238" spans="1:22" ht="13" customHeight="1">
       <c r="A238" s="6" t="s">
         <v>22</v>
       </c>
@@ -15460,8 +16322,11 @@
       <c r="S238" s="13" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="239" spans="1:19" ht="13" customHeight="1">
+      <c r="T238" s="7"/>
+      <c r="U238" s="7"/>
+      <c r="V238" s="7"/>
+    </row>
+    <row r="239" spans="1:22" ht="13" customHeight="1">
       <c r="A239" s="6" t="s">
         <v>22</v>
       </c>
@@ -15474,8 +16339,11 @@
       <c r="S239" s="13" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="240" spans="1:19" ht="13" customHeight="1">
+      <c r="T239" s="7"/>
+      <c r="U239" s="7"/>
+      <c r="V239" s="7"/>
+    </row>
+    <row r="240" spans="1:22" ht="13" customHeight="1">
       <c r="A240" s="6" t="s">
         <v>29</v>
       </c>
@@ -15483,8 +16351,11 @@
         <v>493</v>
       </c>
       <c r="S240"/>
-    </row>
-    <row r="241" spans="1:19" ht="13" customHeight="1">
+      <c r="T240" s="7"/>
+      <c r="U240" s="7"/>
+      <c r="V240" s="7"/>
+    </row>
+    <row r="241" spans="1:22" ht="13" customHeight="1">
       <c r="A241" s="6" t="s">
         <v>50</v>
       </c>
@@ -15519,8 +16390,11 @@
         <v>2703</v>
       </c>
       <c r="S241"/>
-    </row>
-    <row r="242" spans="1:19" ht="13" customHeight="1">
+      <c r="T241" s="7"/>
+      <c r="U241" s="7"/>
+      <c r="V241" s="7"/>
+    </row>
+    <row r="242" spans="1:22" ht="13" customHeight="1">
       <c r="A242" s="6" t="s">
         <v>50</v>
       </c>
@@ -15552,8 +16426,11 @@
         <v>2703</v>
       </c>
       <c r="S242"/>
-    </row>
-    <row r="243" spans="1:19" ht="13" customHeight="1">
+      <c r="T242" s="7"/>
+      <c r="U242" s="7"/>
+      <c r="V242" s="7"/>
+    </row>
+    <row r="243" spans="1:22" ht="13" customHeight="1">
       <c r="A243" s="6" t="s">
         <v>514</v>
       </c>
@@ -15570,8 +16447,11 @@
         <v>2904</v>
       </c>
       <c r="S243"/>
-    </row>
-    <row r="244" spans="1:19" ht="13" customHeight="1">
+      <c r="T243" s="7"/>
+      <c r="U243" s="7"/>
+      <c r="V243" s="7"/>
+    </row>
+    <row r="244" spans="1:22" ht="13" customHeight="1">
       <c r="A244" s="6" t="s">
         <v>517</v>
       </c>
@@ -15591,8 +16471,11 @@
         <v>2228</v>
       </c>
       <c r="S244"/>
-    </row>
-    <row r="245" spans="1:19" ht="13" customHeight="1">
+      <c r="T244" s="7"/>
+      <c r="U244" s="7"/>
+      <c r="V244" s="7"/>
+    </row>
+    <row r="245" spans="1:22" ht="13" customHeight="1">
       <c r="A245" s="6" t="s">
         <v>15</v>
       </c>
@@ -15603,8 +16486,11 @@
         <v>522</v>
       </c>
       <c r="S245"/>
-    </row>
-    <row r="246" spans="1:19" ht="13" customHeight="1">
+      <c r="T245" s="7"/>
+      <c r="U245" s="7"/>
+      <c r="V245" s="7"/>
+    </row>
+    <row r="246" spans="1:22" ht="13" customHeight="1">
       <c r="A246" s="6" t="s">
         <v>50</v>
       </c>
@@ -15639,8 +16525,11 @@
         <v>2700</v>
       </c>
       <c r="S246"/>
-    </row>
-    <row r="247" spans="1:19" ht="13" customHeight="1">
+      <c r="T246" s="7"/>
+      <c r="U246" s="7"/>
+      <c r="V246" s="7"/>
+    </row>
+    <row r="247" spans="1:22" ht="13" customHeight="1">
       <c r="A247" s="6" t="s">
         <v>29</v>
       </c>
@@ -15648,11 +16537,17 @@
         <v>365</v>
       </c>
       <c r="S247"/>
-    </row>
-    <row r="248" spans="1:19" ht="13" customHeight="1">
+      <c r="T247" s="7"/>
+      <c r="U247" s="7"/>
+      <c r="V247" s="7"/>
+    </row>
+    <row r="248" spans="1:22" ht="13" customHeight="1">
       <c r="S248"/>
-    </row>
-    <row r="249" spans="1:19" ht="13" customHeight="1">
+      <c r="T248" s="7"/>
+      <c r="U248" s="7"/>
+      <c r="V248" s="7"/>
+    </row>
+    <row r="249" spans="1:22" ht="13" customHeight="1">
       <c r="A249" s="6" t="s">
         <v>15</v>
       </c>
@@ -15663,8 +16558,11 @@
         <v>2910</v>
       </c>
       <c r="S249"/>
-    </row>
-    <row r="250" spans="1:19" ht="13" customHeight="1">
+      <c r="T249" s="7"/>
+      <c r="U249" s="7"/>
+      <c r="V249" s="7"/>
+    </row>
+    <row r="250" spans="1:22" ht="13" customHeight="1">
       <c r="A250" s="6" t="s">
         <v>15</v>
       </c>
@@ -15675,8 +16573,11 @@
         <v>531</v>
       </c>
       <c r="S250"/>
-    </row>
-    <row r="251" spans="1:19" ht="13" customHeight="1">
+      <c r="T250" s="7"/>
+      <c r="U250" s="7"/>
+      <c r="V250" s="7"/>
+    </row>
+    <row r="251" spans="1:22" ht="13" customHeight="1">
       <c r="A251" s="6" t="s">
         <v>18</v>
       </c>
@@ -15687,8 +16588,11 @@
         <v>533</v>
       </c>
       <c r="S251"/>
-    </row>
-    <row r="252" spans="1:19" ht="13" customHeight="1">
+      <c r="T251" s="7"/>
+      <c r="U251" s="7"/>
+      <c r="V251" s="7"/>
+    </row>
+    <row r="252" spans="1:22" ht="13" customHeight="1">
       <c r="A252" s="6" t="s">
         <v>30</v>
       </c>
@@ -15705,8 +16609,11 @@
         <v>2229</v>
       </c>
       <c r="S252"/>
-    </row>
-    <row r="253" spans="1:19" ht="13" customHeight="1">
+      <c r="T252" s="7"/>
+      <c r="U252" s="7"/>
+      <c r="V252" s="7"/>
+    </row>
+    <row r="253" spans="1:22" ht="13" customHeight="1">
       <c r="A253" s="6" t="s">
         <v>22</v>
       </c>
@@ -15726,8 +16633,11 @@
         <v>2230</v>
       </c>
       <c r="S253"/>
-    </row>
-    <row r="254" spans="1:19" ht="13" customHeight="1">
+      <c r="T253" s="7"/>
+      <c r="U253" s="7"/>
+      <c r="V253" s="7"/>
+    </row>
+    <row r="254" spans="1:22" ht="13" customHeight="1">
       <c r="A254" s="6" t="s">
         <v>118</v>
       </c>
@@ -15747,8 +16657,11 @@
         <v>2921</v>
       </c>
       <c r="S254"/>
-    </row>
-    <row r="255" spans="1:19" ht="13" customHeight="1">
+      <c r="T254" s="7"/>
+      <c r="U254" s="7"/>
+      <c r="V254" s="7"/>
+    </row>
+    <row r="255" spans="1:22" ht="13" customHeight="1">
       <c r="A255" s="6" t="s">
         <v>368</v>
       </c>
@@ -15774,8 +16687,11 @@
         <v>2203</v>
       </c>
       <c r="S255"/>
-    </row>
-    <row r="256" spans="1:19" s="28" customFormat="1" ht="13" customHeight="1">
+      <c r="T255" s="7"/>
+      <c r="U255" s="7"/>
+      <c r="V255" s="7"/>
+    </row>
+    <row r="256" spans="1:22" s="28" customFormat="1" ht="13" customHeight="1">
       <c r="A256" s="28" t="s">
         <v>2566</v>
       </c>
@@ -15810,8 +16726,11 @@
         <v>2232</v>
       </c>
       <c r="S256" s="27"/>
-    </row>
-    <row r="257" spans="1:19" ht="13" customHeight="1">
+      <c r="T256" s="7"/>
+      <c r="U256" s="7"/>
+      <c r="V256" s="7"/>
+    </row>
+    <row r="257" spans="1:22" ht="13" customHeight="1">
       <c r="A257" s="6" t="s">
         <v>118</v>
       </c>
@@ -15831,8 +16750,11 @@
         <v>2935</v>
       </c>
       <c r="S257"/>
-    </row>
-    <row r="258" spans="1:19" ht="13" customHeight="1">
+      <c r="T257" s="7"/>
+      <c r="U257" s="7"/>
+      <c r="V257" s="7"/>
+    </row>
+    <row r="258" spans="1:22" ht="13" customHeight="1">
       <c r="A258" s="6" t="s">
         <v>18</v>
       </c>
@@ -15846,8 +16768,11 @@
         <v>2840</v>
       </c>
       <c r="S258"/>
-    </row>
-    <row r="259" spans="1:19" ht="13" customHeight="1">
+      <c r="T258" s="7"/>
+      <c r="U258" s="7"/>
+      <c r="V258" s="7"/>
+    </row>
+    <row r="259" spans="1:22" ht="13" customHeight="1">
       <c r="A259" s="6" t="s">
         <v>380</v>
       </c>
@@ -15873,8 +16798,11 @@
         <v>2207</v>
       </c>
       <c r="S259"/>
-    </row>
-    <row r="260" spans="1:19" ht="13" customHeight="1">
+      <c r="T259" s="7"/>
+      <c r="U259" s="7"/>
+      <c r="V259" s="7"/>
+    </row>
+    <row r="260" spans="1:22" ht="13" customHeight="1">
       <c r="A260" s="6" t="s">
         <v>130</v>
       </c>
@@ -15891,8 +16819,11 @@
         <v>2208</v>
       </c>
       <c r="S260"/>
-    </row>
-    <row r="261" spans="1:19" ht="13" customHeight="1">
+      <c r="T260" s="7"/>
+      <c r="U260" s="7"/>
+      <c r="V260" s="7"/>
+    </row>
+    <row r="261" spans="1:22" ht="13" customHeight="1">
       <c r="A261" s="6" t="s">
         <v>29</v>
       </c>
@@ -15900,8 +16831,11 @@
         <v>553</v>
       </c>
       <c r="S261"/>
-    </row>
-    <row r="262" spans="1:19" ht="13" customHeight="1">
+      <c r="T261" s="7"/>
+      <c r="U261" s="7"/>
+      <c r="V261" s="7"/>
+    </row>
+    <row r="262" spans="1:22" ht="13" customHeight="1">
       <c r="A262" s="6" t="s">
         <v>118</v>
       </c>
@@ -15921,8 +16855,11 @@
         <v>2936</v>
       </c>
       <c r="S262"/>
-    </row>
-    <row r="263" spans="1:19" ht="13" customHeight="1">
+      <c r="T262" s="7"/>
+      <c r="U262" s="7"/>
+      <c r="V262" s="7"/>
+    </row>
+    <row r="263" spans="1:22" ht="13" customHeight="1">
       <c r="A263" s="6" t="s">
         <v>18</v>
       </c>
@@ -15936,8 +16873,11 @@
         <v>560</v>
       </c>
       <c r="S263"/>
-    </row>
-    <row r="264" spans="1:19" ht="13" customHeight="1">
+      <c r="T263" s="7"/>
+      <c r="U263" s="7"/>
+      <c r="V263" s="7"/>
+    </row>
+    <row r="264" spans="1:22" ht="13" customHeight="1">
       <c r="A264" s="6" t="s">
         <v>391</v>
       </c>
@@ -15963,8 +16903,11 @@
         <v>2207</v>
       </c>
       <c r="S264"/>
-    </row>
-    <row r="265" spans="1:19" ht="13" customHeight="1">
+      <c r="T264" s="7"/>
+      <c r="U264" s="7"/>
+      <c r="V264" s="7"/>
+    </row>
+    <row r="265" spans="1:22" ht="13" customHeight="1">
       <c r="A265" s="6" t="s">
         <v>130</v>
       </c>
@@ -15981,8 +16924,11 @@
         <v>2208</v>
       </c>
       <c r="S265"/>
-    </row>
-    <row r="266" spans="1:19" ht="13" customHeight="1">
+      <c r="T265" s="7"/>
+      <c r="U265" s="7"/>
+      <c r="V265" s="7"/>
+    </row>
+    <row r="266" spans="1:22" ht="13" customHeight="1">
       <c r="A266" s="6" t="s">
         <v>29</v>
       </c>
@@ -15990,8 +16936,11 @@
         <v>559</v>
       </c>
       <c r="S266"/>
-    </row>
-    <row r="267" spans="1:19" ht="13" customHeight="1">
+      <c r="T266" s="7"/>
+      <c r="U266" s="7"/>
+      <c r="V266" s="7"/>
+    </row>
+    <row r="267" spans="1:22" ht="13" customHeight="1">
       <c r="A267" s="6" t="s">
         <v>18</v>
       </c>
@@ -16005,8 +16954,11 @@
         <v>2955</v>
       </c>
       <c r="S267"/>
-    </row>
-    <row r="268" spans="1:19" ht="13" customHeight="1">
+      <c r="T267" s="7"/>
+      <c r="U267" s="7"/>
+      <c r="V267" s="7"/>
+    </row>
+    <row r="268" spans="1:22" ht="13" customHeight="1">
       <c r="A268" s="6" t="s">
         <v>397</v>
       </c>
@@ -16032,8 +16984,11 @@
         <v>2209</v>
       </c>
       <c r="S268"/>
-    </row>
-    <row r="269" spans="1:19" ht="13" customHeight="1">
+      <c r="T268" s="7"/>
+      <c r="U268" s="7"/>
+      <c r="V268" s="7"/>
+    </row>
+    <row r="269" spans="1:22" ht="13" customHeight="1">
       <c r="A269" s="6" t="s">
         <v>130</v>
       </c>
@@ -16050,8 +17005,11 @@
         <v>2208</v>
       </c>
       <c r="S269"/>
-    </row>
-    <row r="270" spans="1:19" ht="13" customHeight="1">
+      <c r="T269" s="7"/>
+      <c r="U269" s="7"/>
+      <c r="V269" s="7"/>
+    </row>
+    <row r="270" spans="1:22" ht="13" customHeight="1">
       <c r="A270" s="6" t="s">
         <v>29</v>
       </c>
@@ -16059,8 +17017,11 @@
         <v>564</v>
       </c>
       <c r="S270"/>
-    </row>
-    <row r="271" spans="1:19" ht="13" customHeight="1">
+      <c r="T270" s="7"/>
+      <c r="U270" s="7"/>
+      <c r="V270" s="7"/>
+    </row>
+    <row r="271" spans="1:22" ht="13" customHeight="1">
       <c r="A271" s="6" t="s">
         <v>118</v>
       </c>
@@ -16080,8 +17041,11 @@
         <v>2923</v>
       </c>
       <c r="S271"/>
-    </row>
-    <row r="272" spans="1:19" ht="13" customHeight="1">
+      <c r="T271" s="7"/>
+      <c r="U271" s="7"/>
+      <c r="V271" s="7"/>
+    </row>
+    <row r="272" spans="1:22" ht="13" customHeight="1">
       <c r="A272" s="6" t="s">
         <v>18</v>
       </c>
@@ -16095,8 +17059,11 @@
         <v>572</v>
       </c>
       <c r="S272"/>
-    </row>
-    <row r="273" spans="1:19" ht="13" customHeight="1">
+      <c r="T272" s="7"/>
+      <c r="U272" s="7"/>
+      <c r="V272" s="7"/>
+    </row>
+    <row r="273" spans="1:22" ht="13" customHeight="1">
       <c r="A273" s="6" t="s">
         <v>380</v>
       </c>
@@ -16122,8 +17089,11 @@
         <v>2207</v>
       </c>
       <c r="S273"/>
-    </row>
-    <row r="274" spans="1:19" ht="13" customHeight="1">
+      <c r="T273" s="7"/>
+      <c r="U273" s="7"/>
+      <c r="V273" s="7"/>
+    </row>
+    <row r="274" spans="1:22" ht="13" customHeight="1">
       <c r="A274" s="6" t="s">
         <v>130</v>
       </c>
@@ -16140,8 +17110,11 @@
         <v>2208</v>
       </c>
       <c r="S274"/>
-    </row>
-    <row r="275" spans="1:19" ht="13" customHeight="1">
+      <c r="T274" s="7"/>
+      <c r="U274" s="7"/>
+      <c r="V274" s="7"/>
+    </row>
+    <row r="275" spans="1:22" ht="13" customHeight="1">
       <c r="A275" s="6" t="s">
         <v>29</v>
       </c>
@@ -16149,8 +17122,11 @@
         <v>571</v>
       </c>
       <c r="S275"/>
-    </row>
-    <row r="276" spans="1:19" ht="13" customHeight="1">
+      <c r="T275" s="7"/>
+      <c r="U275" s="7"/>
+      <c r="V275" s="7"/>
+    </row>
+    <row r="276" spans="1:22" ht="13" customHeight="1">
       <c r="A276" s="6" t="s">
         <v>118</v>
       </c>
@@ -16170,8 +17146,11 @@
         <v>2646</v>
       </c>
       <c r="S276"/>
-    </row>
-    <row r="277" spans="1:19" ht="13" customHeight="1">
+      <c r="T276" s="7"/>
+      <c r="U276" s="7"/>
+      <c r="V276" s="7"/>
+    </row>
+    <row r="277" spans="1:22" ht="13" customHeight="1">
       <c r="A277" s="6" t="s">
         <v>18</v>
       </c>
@@ -16185,8 +17164,11 @@
         <v>579</v>
       </c>
       <c r="S277"/>
-    </row>
-    <row r="278" spans="1:19" ht="13" customHeight="1">
+      <c r="T277" s="7"/>
+      <c r="U277" s="7"/>
+      <c r="V277" s="7"/>
+    </row>
+    <row r="278" spans="1:22" ht="13" customHeight="1">
       <c r="A278" s="6" t="s">
         <v>391</v>
       </c>
@@ -16212,8 +17194,11 @@
         <v>2207</v>
       </c>
       <c r="S278"/>
-    </row>
-    <row r="279" spans="1:19" ht="13" customHeight="1">
+      <c r="T278" s="7"/>
+      <c r="U278" s="7"/>
+      <c r="V278" s="7"/>
+    </row>
+    <row r="279" spans="1:22" ht="13" customHeight="1">
       <c r="A279" s="6" t="s">
         <v>130</v>
       </c>
@@ -16230,8 +17215,11 @@
         <v>2208</v>
       </c>
       <c r="S279"/>
-    </row>
-    <row r="280" spans="1:19" ht="13" customHeight="1">
+      <c r="T279" s="7"/>
+      <c r="U279" s="7"/>
+      <c r="V279" s="7"/>
+    </row>
+    <row r="280" spans="1:22" ht="13" customHeight="1">
       <c r="A280" s="6" t="s">
         <v>29</v>
       </c>
@@ -16239,8 +17227,11 @@
         <v>578</v>
       </c>
       <c r="S280"/>
-    </row>
-    <row r="281" spans="1:19" ht="13" customHeight="1">
+      <c r="T280" s="51"/>
+      <c r="U280" s="51"/>
+      <c r="V280" s="51"/>
+    </row>
+    <row r="281" spans="1:22" ht="13" customHeight="1">
       <c r="A281" s="6" t="s">
         <v>18</v>
       </c>
@@ -16254,8 +17245,11 @@
         <v>584</v>
       </c>
       <c r="S281"/>
-    </row>
-    <row r="282" spans="1:19" ht="13" customHeight="1">
+      <c r="T281" s="51"/>
+      <c r="U281" s="51"/>
+      <c r="V281" s="51"/>
+    </row>
+    <row r="282" spans="1:22" ht="13" customHeight="1">
       <c r="A282" s="6" t="s">
         <v>416</v>
       </c>
@@ -16287,8 +17281,11 @@
         <v>2209</v>
       </c>
       <c r="S282"/>
-    </row>
-    <row r="283" spans="1:19" ht="13" customHeight="1">
+      <c r="T282" s="51"/>
+      <c r="U282" s="51"/>
+      <c r="V282" s="51"/>
+    </row>
+    <row r="283" spans="1:22" ht="13" customHeight="1">
       <c r="A283" s="6" t="s">
         <v>130</v>
       </c>
@@ -16305,8 +17302,11 @@
         <v>2208</v>
       </c>
       <c r="S283"/>
-    </row>
-    <row r="284" spans="1:19" ht="13" customHeight="1">
+      <c r="T283" s="51"/>
+      <c r="U283" s="51"/>
+      <c r="V283" s="51"/>
+    </row>
+    <row r="284" spans="1:22" ht="13" customHeight="1">
       <c r="A284" s="6" t="s">
         <v>29</v>
       </c>
@@ -16314,8 +17314,11 @@
         <v>583</v>
       </c>
       <c r="S284"/>
-    </row>
-    <row r="285" spans="1:19" ht="13" customHeight="1">
+      <c r="T284" s="51"/>
+      <c r="U284" s="51"/>
+      <c r="V284" s="51"/>
+    </row>
+    <row r="285" spans="1:22" ht="13" customHeight="1">
       <c r="A285" s="6" t="s">
         <v>118</v>
       </c>
@@ -16335,8 +17338,11 @@
         <v>2924</v>
       </c>
       <c r="S285"/>
-    </row>
-    <row r="286" spans="1:19" ht="13" customHeight="1">
+      <c r="T285" s="51"/>
+      <c r="U285" s="51"/>
+      <c r="V285" s="51"/>
+    </row>
+    <row r="286" spans="1:22" ht="13" customHeight="1">
       <c r="A286" s="6" t="s">
         <v>590</v>
       </c>
@@ -16356,8 +17362,11 @@
         <v>2237</v>
       </c>
       <c r="S286"/>
-    </row>
-    <row r="287" spans="1:19" ht="13" customHeight="1">
+      <c r="T286" s="7"/>
+      <c r="U286" s="7"/>
+      <c r="V286" s="7"/>
+    </row>
+    <row r="287" spans="1:22" ht="13" customHeight="1">
       <c r="A287" s="6" t="s">
         <v>118</v>
       </c>
@@ -16377,8 +17386,11 @@
         <v>2925</v>
       </c>
       <c r="S287"/>
-    </row>
-    <row r="288" spans="1:19" ht="13" customHeight="1">
+      <c r="T287" s="7"/>
+      <c r="U287" s="7"/>
+      <c r="V287" s="7"/>
+    </row>
+    <row r="288" spans="1:22" ht="13" customHeight="1">
       <c r="A288" s="6" t="s">
         <v>118</v>
       </c>
@@ -16398,8 +17410,11 @@
         <v>2926</v>
       </c>
       <c r="S288"/>
-    </row>
-    <row r="289" spans="1:19" ht="13" customHeight="1">
+      <c r="T288" s="7"/>
+      <c r="U288" s="7"/>
+      <c r="V288" s="7"/>
+    </row>
+    <row r="289" spans="1:22" ht="13" customHeight="1">
       <c r="A289" s="6" t="s">
         <v>590</v>
       </c>
@@ -16419,8 +17434,11 @@
         <v>2238</v>
       </c>
       <c r="S289"/>
-    </row>
-    <row r="290" spans="1:19" ht="13" customHeight="1">
+      <c r="T289" s="7"/>
+      <c r="U289" s="7"/>
+      <c r="V289" s="7"/>
+    </row>
+    <row r="290" spans="1:22" ht="13" customHeight="1">
       <c r="A290" s="6" t="s">
         <v>118</v>
       </c>
@@ -16440,8 +17458,11 @@
         <v>2927</v>
       </c>
       <c r="S290"/>
-    </row>
-    <row r="291" spans="1:19" ht="13" customHeight="1">
+      <c r="T290" s="7"/>
+      <c r="U290" s="7"/>
+      <c r="V290" s="7"/>
+    </row>
+    <row r="291" spans="1:22" ht="13" customHeight="1">
       <c r="A291" s="6" t="s">
         <v>18</v>
       </c>
@@ -16455,8 +17476,11 @@
         <v>541</v>
       </c>
       <c r="S291"/>
-    </row>
-    <row r="292" spans="1:19" ht="13" customHeight="1">
+      <c r="T291" s="7"/>
+      <c r="U291" s="7"/>
+      <c r="V291" s="7"/>
+    </row>
+    <row r="292" spans="1:22" ht="13" customHeight="1">
       <c r="A292" s="6" t="s">
         <v>431</v>
       </c>
@@ -16488,8 +17512,11 @@
         <v>2213</v>
       </c>
       <c r="S292"/>
-    </row>
-    <row r="293" spans="1:19" ht="13" customHeight="1">
+      <c r="T292" s="7"/>
+      <c r="U292" s="7"/>
+      <c r="V292" s="7"/>
+    </row>
+    <row r="293" spans="1:22" ht="13" customHeight="1">
       <c r="A293" s="6" t="s">
         <v>22</v>
       </c>
@@ -16508,8 +17535,11 @@
       <c r="S293" s="13" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="294" spans="1:19" ht="13" customHeight="1">
+      <c r="T293" s="7"/>
+      <c r="U293" s="7"/>
+      <c r="V293" s="7"/>
+    </row>
+    <row r="294" spans="1:22" ht="13" customHeight="1">
       <c r="A294" s="6" t="s">
         <v>29</v>
       </c>
@@ -16517,8 +17547,11 @@
         <v>603</v>
       </c>
       <c r="S294"/>
-    </row>
-    <row r="295" spans="1:19" ht="13" customHeight="1">
+      <c r="T294" s="7"/>
+      <c r="U294" s="7"/>
+      <c r="V294" s="7"/>
+    </row>
+    <row r="295" spans="1:22" ht="13" customHeight="1">
       <c r="A295" s="6" t="s">
         <v>118</v>
       </c>
@@ -16538,8 +17571,11 @@
         <v>2724</v>
       </c>
       <c r="S295"/>
-    </row>
-    <row r="296" spans="1:19" ht="13" customHeight="1">
+      <c r="T295" s="7"/>
+      <c r="U295" s="7"/>
+      <c r="V295" s="7"/>
+    </row>
+    <row r="296" spans="1:22" ht="13" customHeight="1">
       <c r="A296" s="6" t="s">
         <v>50</v>
       </c>
@@ -16574,8 +17610,11 @@
         <v>2700</v>
       </c>
       <c r="S296"/>
-    </row>
-    <row r="297" spans="1:19" ht="13" customHeight="1">
+      <c r="T296" s="7"/>
+      <c r="U296" s="7"/>
+      <c r="V296" s="7"/>
+    </row>
+    <row r="297" spans="1:22" ht="13" customHeight="1">
       <c r="A297" s="6" t="s">
         <v>18</v>
       </c>
@@ -16586,8 +17625,11 @@
         <v>20</v>
       </c>
       <c r="S297"/>
-    </row>
-    <row r="298" spans="1:19" ht="13" customHeight="1">
+      <c r="T297" s="7"/>
+      <c r="U297" s="7"/>
+      <c r="V297" s="7"/>
+    </row>
+    <row r="298" spans="1:22" ht="13" customHeight="1">
       <c r="A298" s="6" t="s">
         <v>431</v>
       </c>
@@ -16619,8 +17661,11 @@
         <v>2213</v>
       </c>
       <c r="S298"/>
-    </row>
-    <row r="299" spans="1:19" ht="13" customHeight="1">
+      <c r="T298" s="7"/>
+      <c r="U298" s="7"/>
+      <c r="V298" s="7"/>
+    </row>
+    <row r="299" spans="1:22" ht="13" customHeight="1">
       <c r="A299" s="6" t="s">
         <v>22</v>
       </c>
@@ -16639,8 +17684,11 @@
       <c r="S299" s="13" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="300" spans="1:19" ht="13" customHeight="1">
+      <c r="T299" s="7"/>
+      <c r="U299" s="7"/>
+      <c r="V299" s="7"/>
+    </row>
+    <row r="300" spans="1:22" ht="13" customHeight="1">
       <c r="A300" s="6" t="s">
         <v>29</v>
       </c>
@@ -16648,8 +17696,11 @@
         <v>614</v>
       </c>
       <c r="S300"/>
-    </row>
-    <row r="301" spans="1:19" ht="13" customHeight="1">
+      <c r="T300" s="7"/>
+      <c r="U300" s="7"/>
+      <c r="V300" s="7"/>
+    </row>
+    <row r="301" spans="1:22" ht="13" customHeight="1">
       <c r="A301" s="6" t="s">
         <v>118</v>
       </c>
@@ -16669,8 +17720,11 @@
         <v>2725</v>
       </c>
       <c r="S301"/>
-    </row>
-    <row r="302" spans="1:19" ht="13" customHeight="1">
+      <c r="T301" s="7"/>
+      <c r="U301" s="7"/>
+      <c r="V301" s="7"/>
+    </row>
+    <row r="302" spans="1:22" ht="13" customHeight="1">
       <c r="A302" s="6" t="s">
         <v>50</v>
       </c>
@@ -16705,8 +17759,11 @@
         <v>2700</v>
       </c>
       <c r="S302"/>
-    </row>
-    <row r="303" spans="1:19" ht="13" customHeight="1">
+      <c r="T302" s="7"/>
+      <c r="U302" s="7"/>
+      <c r="V302" s="7"/>
+    </row>
+    <row r="303" spans="1:22" ht="13" customHeight="1">
       <c r="A303" s="6" t="s">
         <v>18</v>
       </c>
@@ -16720,8 +17777,11 @@
         <v>541</v>
       </c>
       <c r="S303"/>
-    </row>
-    <row r="304" spans="1:19" ht="13" customHeight="1">
+      <c r="T303" s="7"/>
+      <c r="U303" s="7"/>
+      <c r="V303" s="7"/>
+    </row>
+    <row r="304" spans="1:22" ht="13" customHeight="1">
       <c r="A304" s="6" t="s">
         <v>118</v>
       </c>
@@ -16741,8 +17801,11 @@
         <v>2240</v>
       </c>
       <c r="S304"/>
-    </row>
-    <row r="305" spans="1:19" ht="13" customHeight="1">
+      <c r="T304" s="7"/>
+      <c r="U304" s="7"/>
+      <c r="V304" s="7"/>
+    </row>
+    <row r="305" spans="1:22" ht="13" customHeight="1">
       <c r="A305" s="6" t="s">
         <v>22</v>
       </c>
@@ -16755,8 +17818,11 @@
       <c r="S305" s="13" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="306" spans="1:19" ht="13" customHeight="1">
+      <c r="T305" s="7"/>
+      <c r="U305" s="7"/>
+      <c r="V305" s="7"/>
+    </row>
+    <row r="306" spans="1:22" ht="13" customHeight="1">
       <c r="A306" s="6" t="s">
         <v>29</v>
       </c>
@@ -16764,8 +17830,11 @@
         <v>623</v>
       </c>
       <c r="S306"/>
-    </row>
-    <row r="307" spans="1:19" ht="13" customHeight="1">
+      <c r="T306" s="7"/>
+      <c r="U306" s="7"/>
+      <c r="V306" s="7"/>
+    </row>
+    <row r="307" spans="1:22" ht="13" customHeight="1">
       <c r="A307" s="6" t="s">
         <v>50</v>
       </c>
@@ -16800,8 +17869,11 @@
         <v>2701</v>
       </c>
       <c r="S307"/>
-    </row>
-    <row r="308" spans="1:19" ht="13" customHeight="1">
+      <c r="T307" s="7"/>
+      <c r="U307" s="7"/>
+      <c r="V307" s="7"/>
+    </row>
+    <row r="308" spans="1:22" ht="13" customHeight="1">
       <c r="A308" s="6" t="s">
         <v>22</v>
       </c>
@@ -16818,8 +17890,11 @@
         <v>2690</v>
       </c>
       <c r="S308"/>
-    </row>
-    <row r="309" spans="1:19" ht="13" customHeight="1">
+      <c r="T308" s="7"/>
+      <c r="U308" s="7"/>
+      <c r="V308" s="7"/>
+    </row>
+    <row r="309" spans="1:22" ht="13" customHeight="1">
       <c r="A309" s="6" t="s">
         <v>118</v>
       </c>
@@ -16839,8 +17914,11 @@
         <v>2937</v>
       </c>
       <c r="S309"/>
-    </row>
-    <row r="310" spans="1:19" ht="13" customHeight="1">
+      <c r="T309" s="7"/>
+      <c r="U309" s="7"/>
+      <c r="V309" s="7"/>
+    </row>
+    <row r="310" spans="1:22" ht="13" customHeight="1">
       <c r="A310" s="6" t="s">
         <v>118</v>
       </c>
@@ -16860,8 +17938,11 @@
         <v>2933</v>
       </c>
       <c r="S310"/>
-    </row>
-    <row r="311" spans="1:19" ht="13" customHeight="1">
+      <c r="T310" s="7"/>
+      <c r="U310" s="7"/>
+      <c r="V310" s="7"/>
+    </row>
+    <row r="311" spans="1:22" ht="13" customHeight="1">
       <c r="A311" s="6" t="s">
         <v>18</v>
       </c>
@@ -16875,8 +17956,11 @@
         <v>642</v>
       </c>
       <c r="S311"/>
-    </row>
-    <row r="312" spans="1:19" ht="13" customHeight="1">
+      <c r="T311" s="7"/>
+      <c r="U311" s="7"/>
+      <c r="V311" s="7"/>
+    </row>
+    <row r="312" spans="1:22" ht="13" customHeight="1">
       <c r="A312" s="6" t="s">
         <v>495</v>
       </c>
@@ -16908,8 +17992,11 @@
         <v>2213</v>
       </c>
       <c r="S312"/>
-    </row>
-    <row r="313" spans="1:19" ht="13" customHeight="1">
+      <c r="T312" s="7"/>
+      <c r="U312" s="7"/>
+      <c r="V312" s="7"/>
+    </row>
+    <row r="313" spans="1:22" ht="13" customHeight="1">
       <c r="A313" s="6" t="s">
         <v>22</v>
       </c>
@@ -16922,8 +18009,11 @@
       <c r="S313" s="13" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="314" spans="1:19" ht="13" customHeight="1">
+      <c r="T313" s="7"/>
+      <c r="U313" s="7"/>
+      <c r="V313" s="7"/>
+    </row>
+    <row r="314" spans="1:22" ht="13" customHeight="1">
       <c r="A314" s="6" t="s">
         <v>22</v>
       </c>
@@ -16936,8 +18026,11 @@
       <c r="S314" s="13" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="315" spans="1:19" ht="13" customHeight="1">
+      <c r="T314" s="7"/>
+      <c r="U314" s="7"/>
+      <c r="V314" s="7"/>
+    </row>
+    <row r="315" spans="1:22" ht="13" customHeight="1">
       <c r="A315" s="6" t="s">
         <v>22</v>
       </c>
@@ -16950,8 +18043,11 @@
       <c r="S315" s="13" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="316" spans="1:19" ht="13" customHeight="1">
+      <c r="T315" s="7"/>
+      <c r="U315" s="7"/>
+      <c r="V315" s="7"/>
+    </row>
+    <row r="316" spans="1:22" ht="13" customHeight="1">
       <c r="A316" s="6" t="s">
         <v>29</v>
       </c>
@@ -16959,8 +18055,11 @@
         <v>649</v>
       </c>
       <c r="S316"/>
-    </row>
-    <row r="317" spans="1:19" ht="13" customHeight="1">
+      <c r="T316" s="7"/>
+      <c r="U316" s="7"/>
+      <c r="V316" s="7"/>
+    </row>
+    <row r="317" spans="1:22" ht="13" customHeight="1">
       <c r="A317" s="6" t="s">
         <v>50</v>
       </c>
@@ -16995,8 +18094,11 @@
         <v>2733</v>
       </c>
       <c r="S317"/>
-    </row>
-    <row r="318" spans="1:19" ht="13" customHeight="1">
+      <c r="T317" s="7"/>
+      <c r="U317" s="7"/>
+      <c r="V317" s="7"/>
+    </row>
+    <row r="318" spans="1:22" ht="13" customHeight="1">
       <c r="A318" s="6" t="s">
         <v>118</v>
       </c>
@@ -17016,8 +18118,11 @@
         <v>2934</v>
       </c>
       <c r="S318"/>
-    </row>
-    <row r="319" spans="1:19" ht="13" customHeight="1">
+      <c r="T318" s="7"/>
+      <c r="U318" s="7"/>
+      <c r="V318" s="7"/>
+    </row>
+    <row r="319" spans="1:22" ht="13" customHeight="1">
       <c r="A319" s="6" t="s">
         <v>517</v>
       </c>
@@ -17043,8 +18148,11 @@
         <v>2685</v>
       </c>
       <c r="S319"/>
-    </row>
-    <row r="320" spans="1:19" ht="13" customHeight="1">
+      <c r="T319" s="7"/>
+      <c r="U319" s="7"/>
+      <c r="V319" s="7"/>
+    </row>
+    <row r="320" spans="1:22" ht="13" customHeight="1">
       <c r="A320" s="6" t="s">
         <v>50</v>
       </c>
@@ -17079,8 +18187,11 @@
         <v>2700</v>
       </c>
       <c r="S320"/>
-    </row>
-    <row r="321" spans="1:19" ht="13" customHeight="1">
+      <c r="T320" s="7"/>
+      <c r="U320" s="7"/>
+      <c r="V320" s="7"/>
+    </row>
+    <row r="321" spans="1:22" ht="13" customHeight="1">
       <c r="A321" s="6" t="s">
         <v>50</v>
       </c>
@@ -17115,8 +18226,11 @@
         <v>2702</v>
       </c>
       <c r="S321"/>
-    </row>
-    <row r="322" spans="1:19" ht="13" customHeight="1">
+      <c r="T321" s="7"/>
+      <c r="U321" s="7"/>
+      <c r="V321" s="7"/>
+    </row>
+    <row r="322" spans="1:22" ht="13" customHeight="1">
       <c r="A322" s="6" t="s">
         <v>50</v>
       </c>
@@ -17151,8 +18265,11 @@
         <v>2733</v>
       </c>
       <c r="S322"/>
-    </row>
-    <row r="323" spans="1:19" s="28" customFormat="1" ht="13" customHeight="1">
+      <c r="T322" s="7"/>
+      <c r="U322" s="7"/>
+      <c r="V322" s="7"/>
+    </row>
+    <row r="323" spans="1:22" s="28" customFormat="1" ht="13" customHeight="1">
       <c r="A323" s="28" t="s">
         <v>673</v>
       </c>
@@ -17172,8 +18289,11 @@
         <v>2248</v>
       </c>
       <c r="S323" s="27"/>
-    </row>
-    <row r="324" spans="1:19" ht="13" customHeight="1">
+      <c r="T323" s="7"/>
+      <c r="U323" s="7"/>
+      <c r="V323" s="7"/>
+    </row>
+    <row r="324" spans="1:22" ht="13" customHeight="1">
       <c r="A324" s="6" t="s">
         <v>676</v>
       </c>
@@ -17208,8 +18328,11 @@
         <v>2250</v>
       </c>
       <c r="S324"/>
-    </row>
-    <row r="325" spans="1:19" ht="13" customHeight="1">
+      <c r="T324" s="7"/>
+      <c r="U324" s="7"/>
+      <c r="V324" s="7"/>
+    </row>
+    <row r="325" spans="1:22" ht="13" customHeight="1">
       <c r="A325" s="6" t="s">
         <v>118</v>
       </c>
@@ -17234,8 +18357,11 @@
       <c r="S325" s="13" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="326" spans="1:19" ht="13" customHeight="1">
+      <c r="T325" s="7"/>
+      <c r="U325" s="7"/>
+      <c r="V325" s="7"/>
+    </row>
+    <row r="326" spans="1:22" ht="13" customHeight="1">
       <c r="A326" s="6" t="s">
         <v>118</v>
       </c>
@@ -17260,8 +18386,11 @@
       <c r="S326" s="13" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="327" spans="1:19" ht="13" customHeight="1">
+      <c r="T326" s="7"/>
+      <c r="U326" s="7"/>
+      <c r="V326" s="7"/>
+    </row>
+    <row r="327" spans="1:22" ht="13" customHeight="1">
       <c r="A327" s="6" t="s">
         <v>118</v>
       </c>
@@ -17281,8 +18410,11 @@
         <v>2631</v>
       </c>
       <c r="S327"/>
-    </row>
-    <row r="328" spans="1:19" ht="13" customHeight="1">
+      <c r="T327" s="7"/>
+      <c r="U327" s="7"/>
+      <c r="V327" s="7"/>
+    </row>
+    <row r="328" spans="1:22" ht="13" customHeight="1">
       <c r="A328" s="6" t="s">
         <v>118</v>
       </c>
@@ -17302,8 +18434,11 @@
         <v>2632</v>
       </c>
       <c r="S328"/>
-    </row>
-    <row r="329" spans="1:19" ht="13" customHeight="1">
+      <c r="T328" s="7"/>
+      <c r="U328" s="7"/>
+      <c r="V328" s="7"/>
+    </row>
+    <row r="329" spans="1:22" ht="13" customHeight="1">
       <c r="A329" s="6" t="s">
         <v>118</v>
       </c>
@@ -17323,8 +18458,11 @@
         <v>2252</v>
       </c>
       <c r="S329"/>
-    </row>
-    <row r="330" spans="1:19" ht="13" customHeight="1">
+      <c r="T329" s="7"/>
+      <c r="U329" s="7"/>
+      <c r="V329" s="7"/>
+    </row>
+    <row r="330" spans="1:22" ht="13" customHeight="1">
       <c r="A330" s="6" t="s">
         <v>118</v>
       </c>
@@ -17344,8 +18482,11 @@
         <v>2633</v>
       </c>
       <c r="S330"/>
-    </row>
-    <row r="331" spans="1:19" ht="13" customHeight="1">
+      <c r="T330" s="7"/>
+      <c r="U330" s="7"/>
+      <c r="V330" s="7"/>
+    </row>
+    <row r="331" spans="1:22" ht="13" customHeight="1">
       <c r="A331" s="6" t="s">
         <v>18</v>
       </c>
@@ -17359,8 +18500,11 @@
         <v>697</v>
       </c>
       <c r="S331"/>
-    </row>
-    <row r="332" spans="1:19" ht="13" customHeight="1">
+      <c r="T331" s="7"/>
+      <c r="U331" s="7"/>
+      <c r="V331" s="7"/>
+    </row>
+    <row r="332" spans="1:22" ht="13" customHeight="1">
       <c r="A332" s="6" t="s">
         <v>416</v>
       </c>
@@ -17392,8 +18536,11 @@
         <v>2207</v>
       </c>
       <c r="S332"/>
-    </row>
-    <row r="333" spans="1:19" ht="13" customHeight="1">
+      <c r="T332" s="7"/>
+      <c r="U332" s="7"/>
+      <c r="V332" s="7"/>
+    </row>
+    <row r="333" spans="1:22" ht="13" customHeight="1">
       <c r="A333" s="6" t="s">
         <v>130</v>
       </c>
@@ -17410,8 +18557,11 @@
         <v>2208</v>
       </c>
       <c r="S333"/>
-    </row>
-    <row r="334" spans="1:19" ht="13" customHeight="1">
+      <c r="T333" s="7"/>
+      <c r="U333" s="7"/>
+      <c r="V333" s="7"/>
+    </row>
+    <row r="334" spans="1:22" ht="13" customHeight="1">
       <c r="A334" s="6" t="s">
         <v>29</v>
       </c>
@@ -17419,8 +18569,11 @@
         <v>696</v>
       </c>
       <c r="S334"/>
-    </row>
-    <row r="335" spans="1:19" ht="13" customHeight="1">
+      <c r="T334" s="7"/>
+      <c r="U334" s="7"/>
+      <c r="V334" s="7"/>
+    </row>
+    <row r="335" spans="1:22" ht="13" customHeight="1">
       <c r="A335" s="6" t="s">
         <v>118</v>
       </c>
@@ -17441,7 +18594,7 @@
       </c>
       <c r="S335"/>
     </row>
-    <row r="336" spans="1:19" ht="13" customHeight="1">
+    <row r="336" spans="1:22" ht="13" customHeight="1">
       <c r="A336" s="6" t="s">
         <v>118</v>
       </c>

</xml_diff>